<commit_message>
fix: idempotent monoisotopic correction
</commit_message>
<xml_diff>
--- a/test_resources/t_sim/reference/Reference.xlsx
+++ b/test_resources/t_sim/reference/Reference.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25575" windowHeight="9255"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25573" windowHeight="9253"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -976,11 +977,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1304,18 +1306,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="BH20" sqref="BH20"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="24" max="24" width="9.140625" style="2"/>
-    <col min="44" max="44" width="9.140625" customWidth="1"/>
-    <col min="46" max="46" width="9.140625" style="2"/>
+    <col min="24" max="24" width="9.1171875" style="2"/>
+    <col min="44" max="44" width="9.1171875" customWidth="1"/>
+    <col min="46" max="46" width="9.1171875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1403,7 +1405,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>587.53860610000004</v>
       </c>
@@ -1470,7 +1472,7 @@
       <c r="V4">
         <v>159470.20000000001</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4">
         <v>102746</v>
       </c>
       <c r="Y4">
@@ -1540,7 +1542,7 @@
         <f t="shared" si="0"/>
         <v>0.91792821438521288</v>
       </c>
-      <c r="AT4" s="2">
+      <c r="AT4">
         <v>102746</v>
       </c>
       <c r="AU4">
@@ -1611,7 +1613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>615.56964340000002</v>
       </c>
@@ -1678,7 +1680,7 @@
       <c r="V5">
         <v>96046.5</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5">
         <v>62382.7</v>
       </c>
       <c r="Y5">
@@ -1748,7 +1750,7 @@
         <f t="shared" ref="AR5:AR68" si="12">V5/AG5</f>
         <v>0.96439200424127047</v>
       </c>
-      <c r="AT5" s="2">
+      <c r="AT5">
         <v>60181.1</v>
       </c>
       <c r="AU5">
@@ -1807,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="BL5">
-        <f t="shared" ref="BL5:BL68" si="14">T5/BA5</f>
+        <f t="shared" ref="BL5:BL8" si="14">T5/BA5</f>
         <v>1</v>
       </c>
       <c r="BM5">
@@ -1815,11 +1817,11 @@
         <v>1</v>
       </c>
       <c r="BN5">
-        <f t="shared" ref="BN5:BN68" si="15">V5/BC5</f>
+        <f t="shared" ref="BN5:BN8" si="15">V5/BC5</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>643.60097270000006</v>
       </c>
@@ -1886,7 +1888,7 @@
       <c r="V6">
         <v>43827.7</v>
       </c>
-      <c r="X6" s="2">
+      <c r="X6">
         <v>30991.4</v>
       </c>
       <c r="Y6">
@@ -1956,7 +1958,7 @@
         <f t="shared" si="12"/>
         <v>0.96466240546560666</v>
       </c>
-      <c r="AT6" s="2">
+      <c r="AT6">
         <v>29903.1</v>
       </c>
       <c r="AU6">
@@ -2027,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>671.63237379999998</v>
       </c>
@@ -2094,7 +2096,7 @@
       <c r="V7">
         <v>90054</v>
       </c>
-      <c r="X7" s="2">
+      <c r="X7">
         <v>60620.9</v>
       </c>
       <c r="Y7">
@@ -2164,7 +2166,7 @@
         <f t="shared" si="12"/>
         <v>0.96313820446071996</v>
       </c>
-      <c r="AT7" s="2">
+      <c r="AT7">
         <v>58387.5</v>
       </c>
       <c r="AU7">
@@ -2235,7 +2237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>699.66350929999999</v>
       </c>
@@ -2302,7 +2304,7 @@
       <c r="V8">
         <v>140368.4</v>
       </c>
-      <c r="X8" s="2">
+      <c r="X8">
         <v>92171.9</v>
       </c>
       <c r="Y8">
@@ -2372,7 +2374,7 @@
         <f t="shared" si="12"/>
         <v>0.9631610872172649</v>
       </c>
-      <c r="AT8" s="2">
+      <c r="AT8">
         <v>88837.1</v>
       </c>
       <c r="AU8">
@@ -2443,15 +2445,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X9"/>
+      <c r="AT9"/>
+    </row>
+    <row r="10" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X10"/>
+      <c r="AT10"/>
+    </row>
+    <row r="11" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
+      <c r="X11"/>
+      <c r="AT11"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>602.5055132</v>
       </c>
@@ -2518,7 +2530,7 @@
       <c r="V12">
         <v>16653.7</v>
       </c>
-      <c r="X12" s="2">
+      <c r="X12">
         <v>11756.4</v>
       </c>
       <c r="Y12">
@@ -2588,7 +2600,7 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="AT12" s="2">
+      <c r="AT12">
         <v>11756.4</v>
       </c>
       <c r="AU12">
@@ -2623,43 +2635,43 @@
         <v>1</v>
       </c>
       <c r="BF12">
-        <f t="shared" ref="BF12:BF75" si="16">N12/AU12</f>
+        <f t="shared" ref="BF12:BF16" si="16">N12/AU12</f>
         <v>1</v>
       </c>
       <c r="BG12">
-        <f t="shared" ref="BG12:BG75" si="17">O12/AV12</f>
+        <f t="shared" ref="BG12:BG16" si="17">O12/AV12</f>
         <v>1</v>
       </c>
       <c r="BH12">
-        <f t="shared" ref="BH12:BH75" si="18">P12/AW12</f>
+        <f t="shared" ref="BH12:BH16" si="18">P12/AW12</f>
         <v>1</v>
       </c>
       <c r="BI12">
-        <f t="shared" ref="BI12:BI75" si="19">Q12/AX12</f>
+        <f t="shared" ref="BI12:BI16" si="19">Q12/AX12</f>
         <v>1</v>
       </c>
       <c r="BJ12">
-        <f t="shared" ref="BJ12:BJ75" si="20">R12/AY12</f>
+        <f t="shared" ref="BJ12:BJ16" si="20">R12/AY12</f>
         <v>1</v>
       </c>
       <c r="BK12">
-        <f t="shared" ref="BK12:BK75" si="21">S12/AZ12</f>
+        <f t="shared" ref="BK12:BK16" si="21">S12/AZ12</f>
         <v>1</v>
       </c>
       <c r="BL12">
-        <f t="shared" ref="BL12:BL75" si="22">T12/BA12</f>
+        <f t="shared" ref="BL12:BL16" si="22">T12/BA12</f>
         <v>1</v>
       </c>
       <c r="BM12">
-        <f t="shared" ref="BM12:BM75" si="23">U12/BB12</f>
+        <f t="shared" ref="BM12:BM16" si="23">U12/BB12</f>
         <v>1</v>
       </c>
       <c r="BN12">
-        <f t="shared" ref="BN12:BN75" si="24">V12/BC12</f>
+        <f t="shared" ref="BN12:BN16" si="24">V12/BC12</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>630.53617799999995</v>
       </c>
@@ -2726,7 +2738,7 @@
       <c r="V13">
         <v>35219.599999999999</v>
       </c>
-      <c r="X13" s="2">
+      <c r="X13">
         <v>24025.200000000001</v>
       </c>
       <c r="Y13">
@@ -2796,7 +2808,7 @@
         <f t="shared" si="12"/>
         <v>0.98357890503691958</v>
       </c>
-      <c r="AT13" s="2">
+      <c r="AT13">
         <v>23631.599999999999</v>
       </c>
       <c r="AU13">
@@ -2867,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>658.56770849999998</v>
       </c>
@@ -2934,7 +2946,7 @@
       <c r="V14">
         <v>67508.600000000006</v>
       </c>
-      <c r="X14" s="2">
+      <c r="X14">
         <v>45840.7</v>
       </c>
       <c r="Y14">
@@ -3004,7 +3016,7 @@
         <f t="shared" si="12"/>
         <v>0.98184758721695498</v>
       </c>
-      <c r="AT14" s="2">
+      <c r="AT14">
         <v>44991.9</v>
       </c>
       <c r="AU14">
@@ -3075,7 +3087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>682.56713479999996</v>
       </c>
@@ -3142,7 +3154,7 @@
       <c r="V15">
         <v>61007.3</v>
       </c>
-      <c r="X15" s="2">
+      <c r="X15">
         <v>39132.9</v>
       </c>
       <c r="Y15">
@@ -3212,7 +3224,7 @@
         <f t="shared" si="12"/>
         <v>0.98217801697837692</v>
       </c>
-      <c r="AT15" s="2">
+      <c r="AT15">
         <v>38460.6</v>
       </c>
       <c r="AU15">
@@ -3283,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>708.58298219999995</v>
       </c>
@@ -3350,7 +3362,7 @@
       <c r="V16">
         <v>28540.799999999999</v>
       </c>
-      <c r="X16" s="2">
+      <c r="X16">
         <v>20571.2</v>
       </c>
       <c r="Y16">
@@ -3420,7 +3432,7 @@
         <f t="shared" si="12"/>
         <v>0.87904668919147833</v>
       </c>
-      <c r="AT16" s="2">
+      <c r="AT16">
         <v>18794.3</v>
       </c>
       <c r="AU16">
@@ -3491,15 +3503,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X17"/>
+      <c r="AT17"/>
+    </row>
+    <row r="18" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X18"/>
+      <c r="AT18"/>
+    </row>
+    <row r="19" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
       </c>
+      <c r="X19"/>
+      <c r="AT19"/>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>531.34604899999999</v>
       </c>
@@ -3566,7 +3588,7 @@
       <c r="V20">
         <v>31222.6</v>
       </c>
-      <c r="X20" s="2">
+      <c r="X20">
         <v>21620.1</v>
       </c>
       <c r="Y20">
@@ -3636,7 +3658,7 @@
         <f t="shared" si="12"/>
         <v>0.94368295860170037</v>
       </c>
-      <c r="AT20" s="2">
+      <c r="AT20">
         <v>20678.599999999999</v>
       </c>
       <c r="AU20">
@@ -3671,43 +3693,43 @@
         <v>1</v>
       </c>
       <c r="BF20">
-        <f t="shared" ref="BF20:BF83" si="25">N20/AU20</f>
+        <f t="shared" ref="BF20:BF22" si="25">N20/AU20</f>
         <v>1</v>
       </c>
       <c r="BG20">
-        <f t="shared" ref="BG20:BG83" si="26">O20/AV20</f>
+        <f t="shared" ref="BG20:BG22" si="26">O20/AV20</f>
         <v>1</v>
       </c>
       <c r="BH20">
-        <f t="shared" ref="BH20:BH83" si="27">P20/AW20</f>
+        <f t="shared" ref="BH20:BH22" si="27">P20/AW20</f>
         <v>1</v>
       </c>
       <c r="BI20">
-        <f t="shared" ref="BI20:BI83" si="28">Q20/AX20</f>
+        <f t="shared" ref="BI20:BI22" si="28">Q20/AX20</f>
         <v>1</v>
       </c>
       <c r="BJ20">
-        <f t="shared" ref="BJ20:BJ83" si="29">R20/AY20</f>
+        <f t="shared" ref="BJ20:BJ22" si="29">R20/AY20</f>
         <v>1</v>
       </c>
       <c r="BK20">
-        <f t="shared" ref="BK20:BK83" si="30">S20/AZ20</f>
+        <f t="shared" ref="BK20:BK22" si="30">S20/AZ20</f>
         <v>1</v>
       </c>
       <c r="BL20">
-        <f t="shared" ref="BL20:BL83" si="31">T20/BA20</f>
+        <f t="shared" ref="BL20:BL22" si="31">T20/BA20</f>
         <v>1</v>
       </c>
       <c r="BM20">
-        <f t="shared" ref="BM20:BM83" si="32">U20/BB20</f>
+        <f t="shared" ref="BM20:BM22" si="32">U20/BB20</f>
         <v>1</v>
       </c>
       <c r="BN20">
-        <f t="shared" ref="BN20:BN83" si="33">V20/BC20</f>
+        <f t="shared" ref="BN20:BN22" si="33">V20/BC20</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>559.3777</v>
       </c>
@@ -3774,7 +3796,7 @@
       <c r="V21">
         <v>64469.8</v>
       </c>
-      <c r="X21" s="2">
+      <c r="X21">
         <v>43302.9</v>
       </c>
       <c r="Y21">
@@ -3844,7 +3866,7 @@
         <f t="shared" si="12"/>
         <v>0.98812317322326571</v>
       </c>
-      <c r="AT21" s="2">
+      <c r="AT21">
         <v>42820.2</v>
       </c>
       <c r="AU21">
@@ -3915,7 +3937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>587.40924180000002</v>
       </c>
@@ -3982,7 +4004,7 @@
       <c r="V22">
         <v>30543.4</v>
       </c>
-      <c r="X22" s="2">
+      <c r="X22">
         <v>19667.900000000001</v>
       </c>
       <c r="Y22">
@@ -4052,7 +4074,7 @@
         <f t="shared" si="12"/>
         <v>1.092025241781226</v>
       </c>
-      <c r="AT22" s="2">
+      <c r="AT22">
         <v>20323.8</v>
       </c>
       <c r="AU22">
@@ -4123,15 +4145,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X23"/>
+      <c r="AT23"/>
+    </row>
+    <row r="24" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X24"/>
+      <c r="AT24"/>
+    </row>
+    <row r="25" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
       </c>
+      <c r="X25"/>
+      <c r="AT25"/>
     </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>443.29424069999999</v>
       </c>
@@ -4198,7 +4230,7 @@
       <c r="V26">
         <v>28475.5</v>
       </c>
-      <c r="X26" s="2">
+      <c r="X26">
         <v>19393.8</v>
       </c>
       <c r="Y26">
@@ -4268,7 +4300,7 @@
         <f t="shared" si="12"/>
         <v>0.95845155991773778</v>
       </c>
-      <c r="AT26" s="2">
+      <c r="AT26">
         <v>19524.400000000001</v>
       </c>
       <c r="AU26">
@@ -4303,43 +4335,43 @@
         <v>1</v>
       </c>
       <c r="BF26">
-        <f t="shared" ref="BF26:BF89" si="34">N26/AU26</f>
+        <f t="shared" ref="BF26:BF28" si="34">N26/AU26</f>
         <v>1</v>
       </c>
       <c r="BG26">
-        <f t="shared" ref="BG26:BG89" si="35">O26/AV26</f>
+        <f t="shared" ref="BG26:BG28" si="35">O26/AV26</f>
         <v>1</v>
       </c>
       <c r="BH26">
-        <f t="shared" ref="BH26:BH89" si="36">P26/AW26</f>
+        <f t="shared" ref="BH26:BH28" si="36">P26/AW26</f>
         <v>1</v>
       </c>
       <c r="BI26">
-        <f t="shared" ref="BI26:BI89" si="37">Q26/AX26</f>
+        <f t="shared" ref="BI26:BI28" si="37">Q26/AX26</f>
         <v>1</v>
       </c>
       <c r="BJ26">
-        <f t="shared" ref="BJ26:BJ89" si="38">R26/AY26</f>
+        <f t="shared" ref="BJ26:BJ28" si="38">R26/AY26</f>
         <v>1</v>
       </c>
       <c r="BK26">
-        <f t="shared" ref="BK26:BK89" si="39">S26/AZ26</f>
+        <f t="shared" ref="BK26:BK28" si="39">S26/AZ26</f>
         <v>1</v>
       </c>
       <c r="BL26">
-        <f t="shared" ref="BL26:BL89" si="40">T26/BA26</f>
+        <f t="shared" ref="BL26:BL28" si="40">T26/BA26</f>
         <v>1</v>
       </c>
       <c r="BM26">
-        <f t="shared" ref="BM26:BM89" si="41">U26/BB26</f>
+        <f t="shared" ref="BM26:BM28" si="41">U26/BB26</f>
         <v>1</v>
       </c>
       <c r="BN26">
-        <f t="shared" ref="BN26:BN89" si="42">V26/BC26</f>
+        <f t="shared" ref="BN26:BN28" si="42">V26/BC26</f>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>471.32544910000001</v>
       </c>
@@ -4406,7 +4438,7 @@
       <c r="V27">
         <v>73449.8</v>
       </c>
-      <c r="X27" s="2">
+      <c r="X27">
         <v>50801.4</v>
       </c>
       <c r="Y27">
@@ -4476,7 +4508,7 @@
         <f t="shared" si="12"/>
         <v>0.99747405473967821</v>
       </c>
-      <c r="AT27" s="2">
+      <c r="AT27">
         <v>48928.4</v>
       </c>
       <c r="AU27">
@@ -4547,7 +4579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>499.35692669999997</v>
       </c>
@@ -4614,7 +4646,7 @@
       <c r="V28">
         <v>37735.5</v>
       </c>
-      <c r="X28" s="2">
+      <c r="X28">
         <v>24039.8</v>
       </c>
       <c r="Y28">
@@ -4684,7 +4716,7 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="AT28" s="2">
+      <c r="AT28">
         <v>24039.8</v>
       </c>
       <c r="AU28">
@@ -4755,15 +4787,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X29"/>
+      <c r="AT29"/>
+    </row>
+    <row r="30" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X30"/>
+      <c r="AT30"/>
+    </row>
+    <row r="31" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>22</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
       </c>
+      <c r="X31"/>
+      <c r="AT31"/>
     </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>474.28852769999997</v>
       </c>
@@ -4830,7 +4872,7 @@
       <c r="V32">
         <v>17856.7</v>
       </c>
-      <c r="X32" s="2">
+      <c r="X32">
         <v>18092.599999999999</v>
       </c>
       <c r="Y32">
@@ -4900,7 +4942,7 @@
         <f t="shared" si="12"/>
         <v>0.98140158614132389</v>
       </c>
-      <c r="AT32" s="2">
+      <c r="AT32">
         <v>19215.599999999999</v>
       </c>
       <c r="AU32">
@@ -4935,43 +4977,43 @@
         <v>1</v>
       </c>
       <c r="BF32">
-        <f t="shared" ref="BF32:BF94" si="43">N32/AU32</f>
+        <f t="shared" ref="BF32:BF34" si="43">N32/AU32</f>
         <v>1</v>
       </c>
       <c r="BG32">
-        <f t="shared" ref="BG32:BG94" si="44">O32/AV32</f>
+        <f t="shared" ref="BG32:BG34" si="44">O32/AV32</f>
         <v>1</v>
       </c>
       <c r="BH32">
-        <f t="shared" ref="BH32:BH94" si="45">P32/AW32</f>
+        <f t="shared" ref="BH32:BH34" si="45">P32/AW32</f>
         <v>1</v>
       </c>
       <c r="BI32">
-        <f t="shared" ref="BI32:BI94" si="46">Q32/AX32</f>
+        <f t="shared" ref="BI32:BI34" si="46">Q32/AX32</f>
         <v>1</v>
       </c>
       <c r="BJ32">
-        <f t="shared" ref="BJ32:BJ94" si="47">R32/AY32</f>
+        <f t="shared" ref="BJ32:BJ34" si="47">R32/AY32</f>
         <v>1</v>
       </c>
       <c r="BK32">
-        <f t="shared" ref="BK32:BK94" si="48">S32/AZ32</f>
+        <f t="shared" ref="BK32:BK34" si="48">S32/AZ32</f>
         <v>1</v>
       </c>
       <c r="BL32">
-        <f t="shared" ref="BL32:BL94" si="49">T32/BA32</f>
+        <f t="shared" ref="BL32:BL34" si="49">T32/BA32</f>
         <v>1</v>
       </c>
       <c r="BM32">
-        <f t="shared" ref="BM32:BM94" si="50">U32/BB32</f>
+        <f t="shared" ref="BM32:BM34" si="50">U32/BB32</f>
         <v>1</v>
       </c>
       <c r="BN32">
-        <f t="shared" ref="BN32:BN94" si="51">V32/BC32</f>
+        <f t="shared" ref="BN32:BN34" si="51">V32/BC32</f>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>502.32003400000002</v>
       </c>
@@ -5038,7 +5080,7 @@
       <c r="V33">
         <v>41549.5</v>
       </c>
-      <c r="X33" s="2">
+      <c r="X33">
         <v>37924.6</v>
       </c>
       <c r="Y33">
@@ -5108,7 +5150,7 @@
         <f t="shared" si="12"/>
         <v>0.98991489726680126</v>
       </c>
-      <c r="AT33" s="2">
+      <c r="AT33">
         <v>37521.9</v>
       </c>
       <c r="AU33">
@@ -5179,7 +5221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>530.35092550000002</v>
       </c>
@@ -5246,7 +5288,7 @@
       <c r="V34">
         <v>22324.6</v>
       </c>
-      <c r="X34" s="2">
+      <c r="X34">
         <v>23159.8</v>
       </c>
       <c r="Y34">
@@ -5316,7 +5358,7 @@
         <f t="shared" si="12"/>
         <v>0.95661414657348176</v>
       </c>
-      <c r="AT34" s="2">
+      <c r="AT34">
         <v>20931.8</v>
       </c>
       <c r="AU34">
@@ -5387,15 +5429,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X35"/>
+      <c r="AT35"/>
+    </row>
+    <row r="36" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X36"/>
+      <c r="AT36"/>
+    </row>
+    <row r="37" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>22</v>
       </c>
       <c r="B37" t="s">
         <v>69</v>
       </c>
+      <c r="X37"/>
+      <c r="AT37"/>
     </row>
-    <row r="38" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>562.30434790000004</v>
       </c>
@@ -5462,7 +5514,7 @@
       <c r="V38">
         <v>9055.5</v>
       </c>
-      <c r="X38" s="2">
+      <c r="X38">
         <v>10732.6</v>
       </c>
       <c r="Y38">
@@ -5532,7 +5584,7 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="AT38" s="2">
+      <c r="AT38">
         <v>10732.6</v>
       </c>
       <c r="AU38">
@@ -5567,43 +5619,43 @@
         <v>1</v>
       </c>
       <c r="BF38">
-        <f t="shared" ref="BF38:BF94" si="52">N38/AU38</f>
+        <f t="shared" ref="BF38:BF40" si="52">N38/AU38</f>
         <v>1</v>
       </c>
       <c r="BG38">
-        <f t="shared" ref="BG38:BG94" si="53">O38/AV38</f>
+        <f t="shared" ref="BG38:BG40" si="53">O38/AV38</f>
         <v>1</v>
       </c>
       <c r="BH38">
-        <f t="shared" ref="BH38:BH94" si="54">P38/AW38</f>
+        <f t="shared" ref="BH38:BH40" si="54">P38/AW38</f>
         <v>1</v>
       </c>
       <c r="BI38">
-        <f t="shared" ref="BI38:BI94" si="55">Q38/AX38</f>
+        <f t="shared" ref="BI38:BI40" si="55">Q38/AX38</f>
         <v>1</v>
       </c>
       <c r="BJ38">
-        <f t="shared" ref="BJ38:BJ94" si="56">R38/AY38</f>
+        <f t="shared" ref="BJ38:BJ40" si="56">R38/AY38</f>
         <v>1</v>
       </c>
       <c r="BK38">
-        <f t="shared" ref="BK38:BK94" si="57">S38/AZ38</f>
+        <f t="shared" ref="BK38:BK40" si="57">S38/AZ38</f>
         <v>1</v>
       </c>
       <c r="BL38">
-        <f t="shared" ref="BL38:BL94" si="58">T38/BA38</f>
+        <f t="shared" ref="BL38:BL40" si="58">T38/BA38</f>
         <v>1</v>
       </c>
       <c r="BM38">
-        <f t="shared" ref="BM38:BM94" si="59">U38/BB38</f>
+        <f t="shared" ref="BM38:BM40" si="59">U38/BB38</f>
         <v>1</v>
       </c>
       <c r="BN38">
-        <f t="shared" ref="BN38:BN94" si="60">V38/BC38</f>
+        <f t="shared" ref="BN38:BN40" si="60">V38/BC38</f>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>590.33570669999995</v>
       </c>
@@ -5670,7 +5722,7 @@
       <c r="V39">
         <v>23506.6</v>
       </c>
-      <c r="X39" s="2">
+      <c r="X39">
         <v>26730.3</v>
       </c>
       <c r="Y39">
@@ -5740,7 +5792,7 @@
         <f t="shared" si="12"/>
         <v>0.91644736585613074</v>
       </c>
-      <c r="AT39" s="2">
+      <c r="AT39">
         <v>25135.5</v>
       </c>
       <c r="AU39">
@@ -5811,7 +5863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>618.36681739999995</v>
       </c>
@@ -5878,7 +5930,7 @@
       <c r="V40">
         <v>13216.8</v>
       </c>
-      <c r="X40" s="2">
+      <c r="X40">
         <v>14648.3</v>
       </c>
       <c r="Y40">
@@ -5948,7 +6000,7 @@
         <f t="shared" si="12"/>
         <v>0.98770672505660884</v>
       </c>
-      <c r="AT40" s="2">
+      <c r="AT40">
         <v>14505.2</v>
       </c>
       <c r="AU40">
@@ -6019,15 +6071,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X41"/>
+      <c r="AT41"/>
+    </row>
+    <row r="42" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X42"/>
+      <c r="AT42"/>
+    </row>
+    <row r="43" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>22</v>
       </c>
       <c r="B43" t="s">
         <v>76</v>
       </c>
+      <c r="X43"/>
+      <c r="AT43"/>
     </row>
-    <row r="44" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>487.28388280000001</v>
       </c>
@@ -6094,7 +6156,7 @@
       <c r="V44">
         <v>9602.7999999999993</v>
       </c>
-      <c r="X44" s="2">
+      <c r="X44">
         <v>9915</v>
       </c>
       <c r="Y44">
@@ -6164,7 +6226,7 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="AT44" s="2">
+      <c r="AT44">
         <v>9915</v>
       </c>
       <c r="AU44">
@@ -6199,43 +6261,43 @@
         <v>1</v>
       </c>
       <c r="BF44">
-        <f t="shared" ref="BF44:BF94" si="61">N44/AU44</f>
+        <f t="shared" ref="BF44:BF46" si="61">N44/AU44</f>
         <v>1</v>
       </c>
       <c r="BG44">
-        <f t="shared" ref="BG44:BG94" si="62">O44/AV44</f>
+        <f t="shared" ref="BG44:BG46" si="62">O44/AV44</f>
         <v>1</v>
       </c>
       <c r="BH44">
-        <f t="shared" ref="BH44:BH94" si="63">P44/AW44</f>
+        <f t="shared" ref="BH44:BH46" si="63">P44/AW44</f>
         <v>1</v>
       </c>
       <c r="BI44">
-        <f t="shared" ref="BI44:BI94" si="64">Q44/AX44</f>
+        <f t="shared" ref="BI44:BI46" si="64">Q44/AX44</f>
         <v>1</v>
       </c>
       <c r="BJ44">
-        <f t="shared" ref="BJ44:BJ94" si="65">R44/AY44</f>
+        <f t="shared" ref="BJ44:BJ46" si="65">R44/AY44</f>
         <v>1</v>
       </c>
       <c r="BK44">
-        <f t="shared" ref="BK44:BK94" si="66">S44/AZ44</f>
+        <f t="shared" ref="BK44:BK46" si="66">S44/AZ44</f>
         <v>1</v>
       </c>
       <c r="BL44">
-        <f t="shared" ref="BL44:BL94" si="67">T44/BA44</f>
+        <f t="shared" ref="BL44:BL46" si="67">T44/BA44</f>
         <v>1</v>
       </c>
       <c r="BM44">
-        <f t="shared" ref="BM44:BM94" si="68">U44/BB44</f>
+        <f t="shared" ref="BM44:BM46" si="68">U44/BB44</f>
         <v>1</v>
       </c>
       <c r="BN44">
-        <f t="shared" ref="BN44:BN94" si="69">V44/BC44</f>
+        <f t="shared" ref="BN44:BN46" si="69">V44/BC44</f>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>515.31499859999997</v>
       </c>
@@ -6302,7 +6364,7 @@
       <c r="V45">
         <v>22783.5</v>
       </c>
-      <c r="X45" s="2">
+      <c r="X45">
         <v>25300.7</v>
       </c>
       <c r="Y45">
@@ -6372,7 +6434,7 @@
         <f t="shared" si="12"/>
         <v>0.98699942816545083</v>
       </c>
-      <c r="AT45" s="2">
+      <c r="AT45">
         <v>25031.599999999999</v>
       </c>
       <c r="AU45">
@@ -6443,7 +6505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>543.34632790000001</v>
       </c>
@@ -6510,7 +6572,7 @@
       <c r="V46">
         <v>12333.8</v>
       </c>
-      <c r="X46" s="2">
+      <c r="X46">
         <v>12708.2</v>
       </c>
       <c r="Y46">
@@ -6580,7 +6642,7 @@
         <f t="shared" si="12"/>
         <v>0.9829138840630528</v>
       </c>
-      <c r="AT46" s="2">
+      <c r="AT46">
         <v>12441.8</v>
       </c>
       <c r="AU46">
@@ -6651,15 +6713,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X47"/>
+      <c r="AT47"/>
+    </row>
+    <row r="48" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X48"/>
+      <c r="AT48"/>
+    </row>
+    <row r="49" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>22</v>
       </c>
       <c r="B49" t="s">
         <v>83</v>
       </c>
+      <c r="X49"/>
+      <c r="AT49"/>
     </row>
-    <row r="50" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>767.5618273</v>
       </c>
@@ -6726,7 +6798,7 @@
       <c r="V50">
         <v>14876.6</v>
       </c>
-      <c r="X50" s="2">
+      <c r="X50">
         <v>37744.400000000001</v>
       </c>
       <c r="Y50">
@@ -6796,7 +6868,7 @@
         <f t="shared" si="12"/>
         <v>0.29895322362511378</v>
       </c>
-      <c r="AT50" s="2">
+      <c r="AT50">
         <v>9118.2000000000007</v>
       </c>
       <c r="AU50">
@@ -6831,43 +6903,43 @@
         <v>1</v>
       </c>
       <c r="BF50">
-        <f t="shared" ref="BF50:BF94" si="70">N50/AU50</f>
+        <f t="shared" ref="BF50:BF54" si="70">N50/AU50</f>
         <v>1</v>
       </c>
       <c r="BG50">
-        <f t="shared" ref="BG50:BG94" si="71">O50/AV50</f>
+        <f t="shared" ref="BG50:BG54" si="71">O50/AV50</f>
         <v>1</v>
       </c>
       <c r="BH50">
-        <f t="shared" ref="BH50:BH94" si="72">P50/AW50</f>
+        <f t="shared" ref="BH50:BH54" si="72">P50/AW50</f>
         <v>1</v>
       </c>
       <c r="BI50">
-        <f t="shared" ref="BI50:BI94" si="73">Q50/AX50</f>
+        <f t="shared" ref="BI50:BI54" si="73">Q50/AX50</f>
         <v>1</v>
       </c>
       <c r="BJ50">
-        <f t="shared" ref="BJ50:BJ94" si="74">R50/AY50</f>
+        <f t="shared" ref="BJ50:BJ54" si="74">R50/AY50</f>
         <v>1</v>
       </c>
       <c r="BK50">
-        <f t="shared" ref="BK50:BK94" si="75">S50/AZ50</f>
+        <f t="shared" ref="BK50:BK54" si="75">S50/AZ50</f>
         <v>1</v>
       </c>
       <c r="BL50">
-        <f t="shared" ref="BL50:BL94" si="76">T50/BA50</f>
+        <f t="shared" ref="BL50:BL54" si="76">T50/BA50</f>
         <v>1</v>
       </c>
       <c r="BM50">
-        <f t="shared" ref="BM50:BM94" si="77">U50/BB50</f>
+        <f t="shared" ref="BM50:BM54" si="77">U50/BB50</f>
         <v>1</v>
       </c>
       <c r="BN50">
-        <f t="shared" ref="BN50:BN94" si="78">V50/BC50</f>
+        <f t="shared" ref="BN50:BN54" si="78">V50/BC50</f>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>795.5920777</v>
       </c>
@@ -6934,7 +7006,7 @@
       <c r="V51">
         <v>103756</v>
       </c>
-      <c r="X51" s="2">
+      <c r="X51">
         <v>75798.2</v>
       </c>
       <c r="Y51">
@@ -7004,7 +7076,7 @@
         <f t="shared" si="12"/>
         <v>0.98042661919313912</v>
       </c>
-      <c r="AT51" s="2">
+      <c r="AT51">
         <v>74527.7</v>
       </c>
       <c r="AU51">
@@ -7075,7 +7147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>823.62336100000005</v>
       </c>
@@ -7142,7 +7214,7 @@
       <c r="V52">
         <v>163633.9</v>
       </c>
-      <c r="X52" s="2">
+      <c r="X52">
         <v>119782.2</v>
       </c>
       <c r="Y52">
@@ -7212,7 +7284,7 @@
         <f t="shared" si="12"/>
         <v>0.97864179980156096</v>
       </c>
-      <c r="AT52" s="2">
+      <c r="AT52">
         <v>117228.8</v>
       </c>
       <c r="AU52">
@@ -7283,7 +7355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>847.62283769999999</v>
       </c>
@@ -7350,7 +7422,7 @@
       <c r="V53">
         <v>95648.3</v>
       </c>
-      <c r="X53" s="2">
+      <c r="X53">
         <v>70856.600000000006</v>
       </c>
       <c r="Y53">
@@ -7420,7 +7492,7 @@
         <f t="shared" si="12"/>
         <v>0.97697704752595194</v>
       </c>
-      <c r="AT53" s="2">
+      <c r="AT53">
         <v>69528.100000000006</v>
       </c>
       <c r="AU53">
@@ -7491,7 +7563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>873.63868130000003</v>
       </c>
@@ -7558,7 +7630,7 @@
       <c r="V54">
         <v>49959.5</v>
       </c>
-      <c r="X54" s="2">
+      <c r="X54">
         <v>35588.5</v>
       </c>
       <c r="Y54">
@@ -7628,7 +7700,7 @@
         <f t="shared" si="12"/>
         <v>0.9876698192285186</v>
       </c>
-      <c r="AT54" s="2">
+      <c r="AT54">
         <v>35186.699999999997</v>
       </c>
       <c r="AU54">
@@ -7699,15 +7771,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X55"/>
+      <c r="AT55"/>
+    </row>
+    <row r="56" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X56"/>
+      <c r="AT56"/>
+    </row>
+    <row r="57" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
         <v>22</v>
       </c>
       <c r="B57" t="s">
         <v>94</v>
       </c>
+      <c r="X57"/>
+      <c r="AT57"/>
     </row>
-    <row r="58" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>679.50754010000003</v>
       </c>
@@ -7774,7 +7856,7 @@
       <c r="V58">
         <v>33086.5</v>
       </c>
-      <c r="X58" s="2">
+      <c r="X58">
         <v>22359.4</v>
       </c>
       <c r="Y58">
@@ -7844,7 +7926,7 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="AT58" s="2">
+      <c r="AT58">
         <v>22359.4</v>
       </c>
       <c r="AU58">
@@ -7879,43 +7961,43 @@
         <v>1</v>
       </c>
       <c r="BF58">
-        <f t="shared" ref="BF58:BF94" si="79">N58/AU58</f>
+        <f t="shared" ref="BF58:BF62" si="79">N58/AU58</f>
         <v>1</v>
       </c>
       <c r="BG58">
-        <f t="shared" ref="BG58:BG94" si="80">O58/AV58</f>
+        <f t="shared" ref="BG58:BG62" si="80">O58/AV58</f>
         <v>1</v>
       </c>
       <c r="BH58">
-        <f t="shared" ref="BH58:BH94" si="81">P58/AW58</f>
+        <f t="shared" ref="BH58:BH62" si="81">P58/AW58</f>
         <v>1</v>
       </c>
       <c r="BI58">
-        <f t="shared" ref="BI58:BI94" si="82">Q58/AX58</f>
+        <f t="shared" ref="BI58:BI62" si="82">Q58/AX58</f>
         <v>1</v>
       </c>
       <c r="BJ58">
-        <f t="shared" ref="BJ58:BJ94" si="83">R58/AY58</f>
+        <f t="shared" ref="BJ58:BJ62" si="83">R58/AY58</f>
         <v>1</v>
       </c>
       <c r="BK58">
-        <f t="shared" ref="BK58:BK94" si="84">S58/AZ58</f>
+        <f t="shared" ref="BK58:BK62" si="84">S58/AZ58</f>
         <v>1</v>
       </c>
       <c r="BL58">
-        <f t="shared" ref="BL58:BL94" si="85">T58/BA58</f>
+        <f t="shared" ref="BL58:BL62" si="85">T58/BA58</f>
         <v>1</v>
       </c>
       <c r="BM58">
-        <f t="shared" ref="BM58:BM94" si="86">U58/BB58</f>
+        <f t="shared" ref="BM58:BM62" si="86">U58/BB58</f>
         <v>1</v>
       </c>
       <c r="BN58">
-        <f t="shared" ref="BN58:BN94" si="87">V58/BC58</f>
+        <f t="shared" ref="BN58:BN62" si="87">V58/BC58</f>
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>707.53897089999998</v>
       </c>
@@ -7982,7 +8064,7 @@
       <c r="V59">
         <v>58825.9</v>
       </c>
-      <c r="X59" s="2">
+      <c r="X59">
         <v>44087.5</v>
       </c>
       <c r="Y59">
@@ -8052,7 +8134,7 @@
         <f t="shared" si="12"/>
         <v>0.87315445506050771</v>
       </c>
-      <c r="AT59" s="2">
+      <c r="AT59">
         <v>38764.5</v>
       </c>
       <c r="AU59">
@@ -8123,7 +8205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>735.57094710000001</v>
       </c>
@@ -8190,7 +8272,7 @@
       <c r="V60">
         <v>94382.1</v>
       </c>
-      <c r="X60" s="2">
+      <c r="X60">
         <v>67659.5</v>
       </c>
       <c r="Y60">
@@ -8260,7 +8342,7 @@
         <f t="shared" si="12"/>
         <v>0.97995385867714369</v>
       </c>
-      <c r="AT60" s="2">
+      <c r="AT60">
         <v>66318.600000000006</v>
       </c>
       <c r="AU60">
@@ -8331,7 +8413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>759.56996070000002</v>
       </c>
@@ -8398,7 +8480,7 @@
       <c r="V61">
         <v>58514.2</v>
       </c>
-      <c r="X61" s="2">
+      <c r="X61">
         <v>43689.2</v>
       </c>
       <c r="Y61">
@@ -8468,7 +8550,7 @@
         <f t="shared" si="12"/>
         <v>0.98057918894778384</v>
       </c>
-      <c r="AT61" s="2">
+      <c r="AT61">
         <v>42921.599999999999</v>
       </c>
       <c r="AU61">
@@ -8539,7 +8621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>785.58574009999995</v>
       </c>
@@ -8606,7 +8688,7 @@
       <c r="V62">
         <v>27805.4</v>
       </c>
-      <c r="X62" s="2">
+      <c r="X62">
         <v>21191.4</v>
       </c>
       <c r="Y62">
@@ -8676,7 +8758,7 @@
         <f t="shared" si="12"/>
         <v>0.83402521986394229</v>
       </c>
-      <c r="AT62" s="2">
+      <c r="AT62">
         <v>18088.900000000001</v>
       </c>
       <c r="AU62">
@@ -8747,15 +8829,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X63"/>
+      <c r="AT63"/>
+    </row>
+    <row r="64" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X64"/>
+      <c r="AT64"/>
+    </row>
+    <row r="65" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
         <v>22</v>
       </c>
       <c r="B65" t="s">
         <v>105</v>
       </c>
+      <c r="X65"/>
+      <c r="AT65"/>
     </row>
-    <row r="66" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>710.50224560000004</v>
       </c>
@@ -8822,7 +8914,7 @@
       <c r="V66">
         <v>27815.5</v>
       </c>
-      <c r="X66" s="2">
+      <c r="X66">
         <v>23012.2</v>
       </c>
       <c r="Y66">
@@ -8892,7 +8984,7 @@
         <f t="shared" si="12"/>
         <v>0.93214233053176221</v>
       </c>
-      <c r="AT66" s="2">
+      <c r="AT66">
         <v>21506.9</v>
       </c>
       <c r="AU66">
@@ -8927,43 +9019,43 @@
         <v>1</v>
       </c>
       <c r="BF66">
-        <f t="shared" ref="BF66:BF94" si="88">N66/AU66</f>
+        <f t="shared" ref="BF66:BF70" si="88">N66/AU66</f>
         <v>1</v>
       </c>
       <c r="BG66">
-        <f t="shared" ref="BG66:BG94" si="89">O66/AV66</f>
+        <f t="shared" ref="BG66:BG70" si="89">O66/AV66</f>
         <v>1</v>
       </c>
       <c r="BH66">
-        <f t="shared" ref="BH66:BH94" si="90">P66/AW66</f>
+        <f t="shared" ref="BH66:BH70" si="90">P66/AW66</f>
         <v>1</v>
       </c>
       <c r="BI66">
-        <f t="shared" ref="BI66:BI94" si="91">Q66/AX66</f>
+        <f t="shared" ref="BI66:BI70" si="91">Q66/AX66</f>
         <v>1</v>
       </c>
       <c r="BJ66">
-        <f t="shared" ref="BJ66:BJ94" si="92">R66/AY66</f>
+        <f t="shared" ref="BJ66:BJ70" si="92">R66/AY66</f>
         <v>1</v>
       </c>
       <c r="BK66">
-        <f t="shared" ref="BK66:BK94" si="93">S66/AZ66</f>
+        <f t="shared" ref="BK66:BK70" si="93">S66/AZ66</f>
         <v>1</v>
       </c>
       <c r="BL66">
-        <f t="shared" ref="BL66:BL94" si="94">T66/BA66</f>
+        <f t="shared" ref="BL66:BL70" si="94">T66/BA66</f>
         <v>1</v>
       </c>
       <c r="BM66">
-        <f t="shared" ref="BM66:BM94" si="95">U66/BB66</f>
+        <f t="shared" ref="BM66:BM70" si="95">U66/BB66</f>
         <v>1</v>
       </c>
       <c r="BN66">
-        <f t="shared" ref="BN66:BN94" si="96">V66/BC66</f>
+        <f t="shared" ref="BN66:BN70" si="96">V66/BC66</f>
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>738.53363260000003</v>
       </c>
@@ -9030,7 +9122,7 @@
       <c r="V67">
         <v>52762.400000000001</v>
       </c>
-      <c r="X67" s="2">
+      <c r="X67">
         <v>43817.2</v>
       </c>
       <c r="Y67">
@@ -9100,7 +9192,7 @@
         <f t="shared" si="12"/>
         <v>0.98266996195027645</v>
       </c>
-      <c r="AT67" s="2">
+      <c r="AT67">
         <v>43097.1</v>
       </c>
       <c r="AU67">
@@ -9171,7 +9263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>766.56472970000004</v>
       </c>
@@ -9238,7 +9330,7 @@
       <c r="V68">
         <v>78107.100000000006</v>
       </c>
-      <c r="X68" s="2">
+      <c r="X68">
         <v>61106.1</v>
       </c>
       <c r="Y68">
@@ -9308,7 +9400,7 @@
         <f t="shared" si="12"/>
         <v>0.9817629905226376</v>
       </c>
-      <c r="AT68" s="2">
+      <c r="AT68">
         <v>59996.4</v>
       </c>
       <c r="AU68">
@@ -9379,7 +9471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>790.56461779999995</v>
       </c>
@@ -9446,7 +9538,7 @@
       <c r="V69">
         <v>57116</v>
       </c>
-      <c r="X69" s="2">
+      <c r="X69">
         <v>42407.8</v>
       </c>
       <c r="Y69">
@@ -9516,7 +9608,7 @@
         <f t="shared" ref="AR69:AR94" si="106">V69/AG69</f>
         <v>0.98148249979379176</v>
       </c>
-      <c r="AT69" s="2">
+      <c r="AT69">
         <v>41650</v>
       </c>
       <c r="AU69">
@@ -9587,7 +9679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>816.5801841</v>
       </c>
@@ -9654,7 +9746,7 @@
       <c r="V70">
         <v>26816.799999999999</v>
       </c>
-      <c r="X70" s="2">
+      <c r="X70">
         <v>21949.4</v>
       </c>
       <c r="Y70">
@@ -9724,7 +9816,7 @@
         <f t="shared" si="106"/>
         <v>0.98186158566501414</v>
       </c>
-      <c r="AT70" s="2">
+      <c r="AT70">
         <v>21637.4</v>
       </c>
       <c r="AU70">
@@ -9795,290 +9887,300 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X71"/>
+      <c r="AT71"/>
+    </row>
+    <row r="72" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X72"/>
+      <c r="AT72"/>
+    </row>
+    <row r="73" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
         <v>22</v>
       </c>
       <c r="B73" t="s">
         <v>116</v>
       </c>
+      <c r="X73"/>
+      <c r="AT73"/>
     </row>
-    <row r="74" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A74">
+    <row r="74" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A74" s="4">
         <v>798.51794659999996</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="4">
         <v>31</v>
       </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-      <c r="G74" t="s">
+      <c r="E74" s="4">
+        <v>1</v>
+      </c>
+      <c r="F74" s="4">
+        <v>0</v>
+      </c>
+      <c r="G74" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H74" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J74">
+      <c r="J74" s="4">
         <v>-0.87</v>
       </c>
-      <c r="K74">
-        <v>0</v>
-      </c>
-      <c r="L74">
-        <v>0</v>
-      </c>
-      <c r="M74">
+      <c r="K74" s="4">
+        <v>0</v>
+      </c>
+      <c r="L74" s="4">
+        <v>0</v>
+      </c>
+      <c r="M74" s="4">
         <v>18042.5</v>
       </c>
-      <c r="N74">
+      <c r="N74" s="4">
         <v>21808.2</v>
       </c>
-      <c r="O74">
+      <c r="O74" s="4">
         <v>28465.5</v>
       </c>
-      <c r="P74">
+      <c r="P74" s="4">
         <v>23815.1</v>
       </c>
-      <c r="Q74">
+      <c r="Q74" s="4">
         <v>46383.6</v>
       </c>
-      <c r="R74">
+      <c r="R74" s="4">
         <v>28927</v>
       </c>
-      <c r="S74">
+      <c r="S74" s="4">
         <v>35127.199999999997</v>
       </c>
-      <c r="T74">
+      <c r="T74" s="4">
         <v>45733.5</v>
       </c>
-      <c r="U74">
+      <c r="U74" s="4">
         <v>12634</v>
       </c>
-      <c r="V74">
+      <c r="V74" s="4">
         <v>20618.599999999999</v>
       </c>
-      <c r="X74" s="2">
-        <v>30157.3</v>
+      <c r="X74">
+        <v>18387.2</v>
       </c>
       <c r="Y74">
-        <v>36423.599999999999</v>
+        <v>22207.9</v>
       </c>
       <c r="Z74">
-        <v>47765.599999999999</v>
+        <v>29123.200000000001</v>
       </c>
       <c r="AA74">
-        <v>39963.800000000003</v>
+        <v>24366.400000000001</v>
       </c>
       <c r="AB74">
-        <v>77461.7</v>
+        <v>47229.2</v>
       </c>
       <c r="AC74">
-        <v>48340</v>
+        <v>29473.4</v>
       </c>
       <c r="AD74">
-        <v>58461.9</v>
+        <v>35644.9</v>
       </c>
       <c r="AE74">
-        <v>76482.600000000006</v>
+        <v>46632.3</v>
       </c>
       <c r="AF74">
-        <v>21105.4</v>
+        <v>12868.2</v>
       </c>
       <c r="AG74">
-        <v>34551.199999999997</v>
-      </c>
-      <c r="AI74">
+        <v>21066.3</v>
+      </c>
+      <c r="AI74" s="4">
         <f t="shared" si="97"/>
-        <v>0.59827968684199184</v>
-      </c>
-      <c r="AJ74">
+        <v>0.98125326313957528</v>
+      </c>
+      <c r="AJ74" s="4">
         <f t="shared" si="98"/>
-        <v>0.59873818073995988</v>
-      </c>
-      <c r="AK74">
+        <v>0.9820019002246948</v>
+      </c>
+      <c r="AK74" s="4">
         <f t="shared" si="99"/>
-        <v>0.5959414306530223</v>
-      </c>
-      <c r="AL74">
+        <v>0.97741663004065482</v>
+      </c>
+      <c r="AL74" s="4">
         <f t="shared" si="100"/>
-        <v>0.59591680470826092</v>
-      </c>
-      <c r="AM74">
+        <v>0.97737458139076749</v>
+      </c>
+      <c r="AM74" s="4">
         <f t="shared" si="101"/>
-        <v>0.59879398464015121</v>
-      </c>
-      <c r="AN74">
+        <v>0.9820958220761733</v>
+      </c>
+      <c r="AN74" s="4">
         <f t="shared" si="102"/>
-        <v>0.59840711625982623</v>
-      </c>
-      <c r="AO74">
+        <v>0.98146124980490879</v>
+      </c>
+      <c r="AO74" s="4">
         <f t="shared" si="103"/>
-        <v>0.60085628417824255</v>
-      </c>
-      <c r="AP74">
+        <v>0.98547618312858209</v>
+      </c>
+      <c r="AP74" s="4">
         <f t="shared" si="104"/>
-        <v>0.59795953589443873</v>
-      </c>
-      <c r="AQ74">
+        <v>0.98072580593279757</v>
+      </c>
+      <c r="AQ74" s="4">
         <f t="shared" si="105"/>
-        <v>0.59861457257384365</v>
-      </c>
-      <c r="AR74">
+        <v>0.98180009636157339</v>
+      </c>
+      <c r="AR74" s="4">
         <f t="shared" si="106"/>
-        <v>0.59675496075389567</v>
-      </c>
-      <c r="AT74" s="2">
-        <v>29591.9</v>
+        <v>0.9787480478299464</v>
+      </c>
+      <c r="AT74">
+        <v>18042.5</v>
       </c>
       <c r="AU74">
-        <v>35768.1</v>
+        <v>21808.2</v>
       </c>
       <c r="AV74">
-        <v>46686.9</v>
+        <v>28465.5</v>
       </c>
       <c r="AW74">
-        <v>39059.699999999997</v>
+        <v>23815.1</v>
       </c>
       <c r="AX74">
-        <v>76074.7</v>
+        <v>46383.6</v>
       </c>
       <c r="AY74">
-        <v>47443.9</v>
+        <v>28927</v>
       </c>
       <c r="AZ74">
-        <v>57612.800000000003</v>
+        <v>35127.199999999997</v>
       </c>
       <c r="BA74">
-        <v>75008.5</v>
+        <v>45733.5</v>
       </c>
       <c r="BB74">
-        <v>20721.3</v>
+        <v>12634</v>
       </c>
       <c r="BC74">
-        <v>33817.1</v>
-      </c>
-      <c r="BE74">
+        <v>20618.599999999999</v>
+      </c>
+      <c r="BE74" s="4">
         <f t="shared" si="107"/>
-        <v>0.60971076544594971</v>
-      </c>
-      <c r="BF74">
-        <f t="shared" ref="BF74:BF94" si="108">N74/AU74</f>
-        <v>0.60971088763451231</v>
-      </c>
-      <c r="BG74">
-        <f t="shared" ref="BG74:BG94" si="109">O74/AV74</f>
-        <v>0.60971064688381538</v>
-      </c>
-      <c r="BH74">
-        <f t="shared" ref="BH74:BH94" si="110">P74/AW74</f>
-        <v>0.60971026403172579</v>
-      </c>
-      <c r="BI74">
-        <f t="shared" ref="BI74:BI94" si="111">Q74/AX74</f>
-        <v>0.60971124434273161</v>
-      </c>
-      <c r="BJ74">
-        <f t="shared" ref="BJ74:BJ94" si="112">R74/AY74</f>
-        <v>0.60970957277964077</v>
-      </c>
-      <c r="BK74">
-        <f t="shared" ref="BK74:BK94" si="113">S74/AZ74</f>
-        <v>0.60971173072650509</v>
-      </c>
-      <c r="BL74">
-        <f t="shared" ref="BL74:BL94" si="114">T74/BA74</f>
-        <v>0.60971089943139778</v>
-      </c>
-      <c r="BM74">
-        <f t="shared" ref="BM74:BM94" si="115">U74/BB74</f>
-        <v>0.60971078069426143</v>
-      </c>
-      <c r="BN74">
-        <f t="shared" ref="BN74:BN94" si="116">V74/BC74</f>
-        <v>0.60970928908747346</v>
+        <v>1</v>
+      </c>
+      <c r="BF74" s="4">
+        <f t="shared" ref="BF74:BF78" si="108">N74/AU74</f>
+        <v>1</v>
+      </c>
+      <c r="BG74" s="4">
+        <f t="shared" ref="BG74:BG78" si="109">O74/AV74</f>
+        <v>1</v>
+      </c>
+      <c r="BH74" s="4">
+        <f t="shared" ref="BH74:BH78" si="110">P74/AW74</f>
+        <v>1</v>
+      </c>
+      <c r="BI74" s="4">
+        <f t="shared" ref="BI74:BI78" si="111">Q74/AX74</f>
+        <v>1</v>
+      </c>
+      <c r="BJ74" s="4">
+        <f t="shared" ref="BJ74:BJ78" si="112">R74/AY74</f>
+        <v>1</v>
+      </c>
+      <c r="BK74" s="4">
+        <f t="shared" ref="BK74:BK78" si="113">S74/AZ74</f>
+        <v>1</v>
+      </c>
+      <c r="BL74" s="4">
+        <f t="shared" ref="BL74:BL78" si="114">T74/BA74</f>
+        <v>1</v>
+      </c>
+      <c r="BM74" s="4">
+        <f t="shared" ref="BM74:BM78" si="115">U74/BB74</f>
+        <v>1</v>
+      </c>
+      <c r="BN74" s="4">
+        <f t="shared" ref="BN74:BN78" si="116">V74/BC74</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A75">
+    <row r="75" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A75" s="4">
         <v>826.54853979999996</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="4">
         <v>33</v>
       </c>
-      <c r="E75">
-        <v>1</v>
-      </c>
-      <c r="F75">
-        <v>0</v>
-      </c>
-      <c r="G75" t="s">
+      <c r="E75" s="4">
+        <v>1</v>
+      </c>
+      <c r="F75" s="4">
+        <v>0</v>
+      </c>
+      <c r="G75" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H75" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I75" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J75">
+      <c r="J75" s="4">
         <v>-1.69</v>
       </c>
-      <c r="K75">
-        <v>0</v>
-      </c>
-      <c r="L75">
-        <v>0</v>
-      </c>
-      <c r="M75">
+      <c r="K75" s="4">
+        <v>0</v>
+      </c>
+      <c r="L75" s="4">
+        <v>0</v>
+      </c>
+      <c r="M75" s="4">
         <v>34838.1</v>
       </c>
-      <c r="N75">
+      <c r="N75" s="4">
         <v>41525</v>
       </c>
-      <c r="O75">
-        <v>0</v>
-      </c>
-      <c r="P75">
-        <v>0</v>
-      </c>
-      <c r="Q75">
+      <c r="O75" s="4">
+        <v>0</v>
+      </c>
+      <c r="P75" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="4">
         <v>78073.100000000006</v>
       </c>
-      <c r="R75">
+      <c r="R75" s="4">
         <v>47568.7</v>
       </c>
-      <c r="S75">
+      <c r="S75" s="4">
         <v>32722.3</v>
       </c>
-      <c r="T75">
+      <c r="T75" s="4">
         <v>42651.199999999997</v>
       </c>
-      <c r="U75">
+      <c r="U75" s="4">
         <v>25694</v>
       </c>
-      <c r="V75">
+      <c r="V75" s="4">
         <v>43184.2</v>
       </c>
-      <c r="X75" s="2">
+      <c r="X75">
         <v>40344.300000000003</v>
       </c>
       <c r="Y75">
@@ -10108,51 +10210,51 @@
       <c r="AG75">
         <v>44388.6</v>
       </c>
-      <c r="AI75">
+      <c r="AI75" s="4">
         <f t="shared" si="97"/>
         <v>0.86351975371985623</v>
       </c>
-      <c r="AJ75">
+      <c r="AJ75" s="4">
         <f t="shared" si="98"/>
         <v>0.87794224292307732</v>
       </c>
-      <c r="AK75" t="e">
+      <c r="AK75" s="4" t="e">
         <f t="shared" si="99"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AL75" t="e">
+      <c r="AL75" s="4" t="e">
         <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AM75">
+      <c r="AM75" s="4">
         <f t="shared" si="101"/>
         <v>0.87412221774374144</v>
       </c>
-      <c r="AN75">
+      <c r="AN75" s="4">
         <f t="shared" si="102"/>
         <v>0.95769285747361088</v>
       </c>
-      <c r="AO75">
+      <c r="AO75" s="4">
         <f t="shared" si="103"/>
         <v>1.1634057803550413</v>
       </c>
-      <c r="AP75">
+      <c r="AP75" s="4">
         <f t="shared" si="104"/>
         <v>0.93114725466652104</v>
       </c>
-      <c r="AQ75">
+      <c r="AQ75" s="4">
         <f t="shared" si="105"/>
         <v>0.97236624003754135</v>
       </c>
-      <c r="AR75">
+      <c r="AR75" s="4">
         <f t="shared" si="106"/>
         <v>0.97286690726898339</v>
       </c>
-      <c r="AT75" s="2">
-        <v>58466.2</v>
+      <c r="AT75">
+        <v>34838.1</v>
       </c>
       <c r="AU75">
-        <v>69688.399999999994</v>
+        <v>41525</v>
       </c>
       <c r="AV75">
         <v>0</v>
@@ -10161,132 +10263,132 @@
         <v>0</v>
       </c>
       <c r="AX75">
-        <v>131024.4</v>
+        <v>78073.100000000006</v>
       </c>
       <c r="AY75">
-        <v>79831</v>
+        <v>47568.7</v>
       </c>
       <c r="AZ75">
-        <v>54915.5</v>
+        <v>32722.3</v>
       </c>
       <c r="BA75">
-        <v>71578.3</v>
+        <v>42651.199999999997</v>
       </c>
       <c r="BB75">
-        <v>43120.4</v>
+        <v>25694</v>
       </c>
       <c r="BC75">
-        <v>72472.899999999994</v>
-      </c>
-      <c r="BE75">
+        <v>43184.2</v>
+      </c>
+      <c r="BE75" s="4">
         <f t="shared" si="107"/>
-        <v>0.59586735583978434</v>
-      </c>
-      <c r="BF75">
+        <v>1</v>
+      </c>
+      <c r="BF75" s="4">
         <f t="shared" si="108"/>
-        <v>0.59586674396312733</v>
-      </c>
-      <c r="BG75" t="e">
+        <v>1</v>
+      </c>
+      <c r="BG75" s="4" t="e">
         <f t="shared" si="109"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BH75" t="e">
+      <c r="BH75" s="4" t="e">
         <f t="shared" si="110"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="BI75">
+      <c r="BI75" s="4">
         <f t="shared" si="111"/>
-        <v>0.59586687670388117</v>
-      </c>
-      <c r="BJ75">
+        <v>1</v>
+      </c>
+      <c r="BJ75" s="4">
         <f t="shared" si="112"/>
-        <v>0.59586752013628785</v>
-      </c>
-      <c r="BK75">
+        <v>1</v>
+      </c>
+      <c r="BK75" s="4">
         <f t="shared" si="113"/>
-        <v>0.59586637652393226</v>
-      </c>
-      <c r="BL75">
+        <v>1</v>
+      </c>
+      <c r="BL75" s="4">
         <f t="shared" si="114"/>
-        <v>0.5958677420391375</v>
-      </c>
-      <c r="BM75">
+        <v>1</v>
+      </c>
+      <c r="BM75" s="4">
         <f t="shared" si="115"/>
-        <v>0.59586645763953949</v>
-      </c>
-      <c r="BN75">
+        <v>1</v>
+      </c>
+      <c r="BN75" s="4">
         <f t="shared" si="116"/>
-        <v>0.59586686885718665</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A76">
+    <row r="76" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A76" s="4">
         <v>854.58128160000001</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="4">
         <v>35</v>
       </c>
-      <c r="E76">
-        <v>1</v>
-      </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-      <c r="G76" t="s">
+      <c r="E76" s="4">
+        <v>1</v>
+      </c>
+      <c r="F76" s="4">
+        <v>0</v>
+      </c>
+      <c r="G76" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I76" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J76">
+      <c r="J76" s="4">
         <v>0.05</v>
       </c>
-      <c r="K76">
-        <v>0</v>
-      </c>
-      <c r="L76">
-        <v>0</v>
-      </c>
-      <c r="M76">
+      <c r="K76" s="4">
+        <v>0</v>
+      </c>
+      <c r="L76" s="4">
+        <v>0</v>
+      </c>
+      <c r="M76" s="4">
         <v>54177.4</v>
       </c>
-      <c r="N76">
+      <c r="N76" s="4">
         <v>66905.3</v>
       </c>
-      <c r="O76">
+      <c r="O76" s="4">
         <v>46972</v>
       </c>
-      <c r="P76">
+      <c r="P76" s="4">
         <v>46194.2</v>
       </c>
-      <c r="Q76">
+      <c r="Q76" s="4">
         <v>118376.7</v>
       </c>
-      <c r="R76">
+      <c r="R76" s="4">
         <v>71684.899999999994</v>
       </c>
-      <c r="S76">
+      <c r="S76" s="4">
         <v>72269</v>
       </c>
-      <c r="T76">
+      <c r="T76" s="4">
         <v>95559.2</v>
       </c>
-      <c r="U76">
+      <c r="U76" s="4">
         <v>39203.1</v>
       </c>
-      <c r="V76">
+      <c r="V76" s="4">
         <v>64930.5</v>
       </c>
-      <c r="X76" s="2">
+      <c r="X76">
         <v>56144.4</v>
       </c>
       <c r="Y76">
@@ -10316,118 +10418,118 @@
       <c r="AG76">
         <v>67513.3</v>
       </c>
-      <c r="AI76">
+      <c r="AI76" s="4">
         <f t="shared" si="97"/>
         <v>0.96496533937489759</v>
       </c>
-      <c r="AJ76">
+      <c r="AJ76" s="4">
         <f t="shared" si="98"/>
         <v>0.96373947388890646</v>
       </c>
-      <c r="AK76">
+      <c r="AK76" s="4">
         <f t="shared" si="99"/>
         <v>1.7191125555384761</v>
       </c>
-      <c r="AL76">
+      <c r="AL76" s="4">
         <f t="shared" si="100"/>
         <v>1.5000405906096059</v>
       </c>
-      <c r="AM76">
+      <c r="AM76" s="4">
         <f t="shared" si="101"/>
         <v>0.95656238838582264</v>
       </c>
-      <c r="AN76">
+      <c r="AN76" s="4">
         <f t="shared" si="102"/>
         <v>0.94737335958872415</v>
       </c>
-      <c r="AO76">
+      <c r="AO76" s="4">
         <f t="shared" si="103"/>
         <v>1.0708231835612216</v>
       </c>
-      <c r="AP76">
+      <c r="AP76" s="4">
         <f t="shared" si="104"/>
         <v>1.0125403043368155</v>
       </c>
-      <c r="AQ76">
+      <c r="AQ76" s="4">
         <f t="shared" si="105"/>
         <v>0.96288282004111569</v>
       </c>
-      <c r="AR76">
+      <c r="AR76" s="4">
         <f t="shared" si="106"/>
         <v>0.96174383417785825</v>
       </c>
-      <c r="AT76" s="2">
-        <v>93034.3</v>
+      <c r="AT76">
+        <v>54177.4</v>
       </c>
       <c r="AU76">
-        <v>114890.9</v>
+        <v>66905.3</v>
       </c>
       <c r="AV76">
-        <v>80661.100000000006</v>
+        <v>46972</v>
       </c>
       <c r="AW76">
-        <v>79325.5</v>
+        <v>46194.2</v>
       </c>
       <c r="AX76">
-        <v>203278.4</v>
+        <v>118376.7</v>
       </c>
       <c r="AY76">
-        <v>123098.6</v>
+        <v>71684.899999999994</v>
       </c>
       <c r="AZ76">
-        <v>124101.6</v>
+        <v>72269</v>
       </c>
       <c r="BA76">
-        <v>164096</v>
+        <v>95559.2</v>
       </c>
       <c r="BB76">
-        <v>67320.3</v>
+        <v>39203.1</v>
       </c>
       <c r="BC76">
-        <v>111499.8</v>
-      </c>
-      <c r="BE76">
+        <v>64930.5</v>
+      </c>
+      <c r="BE76" s="4">
         <f t="shared" si="107"/>
-        <v>0.58233791193140594</v>
-      </c>
-      <c r="BF76">
+        <v>1</v>
+      </c>
+      <c r="BF76" s="4">
         <f t="shared" si="108"/>
-        <v>0.58233767861510355</v>
-      </c>
-      <c r="BG76">
+        <v>1</v>
+      </c>
+      <c r="BG76" s="4">
         <f t="shared" si="109"/>
-        <v>0.58233770677563279</v>
-      </c>
-      <c r="BH76">
+        <v>1</v>
+      </c>
+      <c r="BH76" s="4">
         <f t="shared" si="110"/>
-        <v>0.58233733162728252</v>
-      </c>
-      <c r="BI76">
+        <v>1</v>
+      </c>
+      <c r="BI76" s="4">
         <f t="shared" si="111"/>
-        <v>0.58233781847948429</v>
-      </c>
-      <c r="BJ76">
+        <v>1</v>
+      </c>
+      <c r="BJ76" s="4">
         <f t="shared" si="112"/>
-        <v>0.58233724835213385</v>
-      </c>
-      <c r="BK76">
+        <v>1</v>
+      </c>
+      <c r="BK76" s="4">
         <f t="shared" si="113"/>
-        <v>0.58233737518291462</v>
-      </c>
-      <c r="BL76">
+        <v>1</v>
+      </c>
+      <c r="BL76" s="4">
         <f t="shared" si="114"/>
-        <v>0.58233716848673944</v>
-      </c>
-      <c r="BM76">
+        <v>1</v>
+      </c>
+      <c r="BM76" s="4">
         <f t="shared" si="115"/>
-        <v>0.58233697710794508</v>
-      </c>
-      <c r="BN76">
+        <v>1</v>
+      </c>
+      <c r="BN76" s="4">
         <f t="shared" si="116"/>
-        <v>0.58233736742128683</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>878.57993999999997</v>
       </c>
@@ -10494,7 +10596,7 @@
       <c r="V77">
         <v>41225.800000000003</v>
       </c>
-      <c r="X77" s="2">
+      <c r="X77">
         <v>36914.300000000003</v>
       </c>
       <c r="Y77">
@@ -10564,7 +10666,7 @@
         <f t="shared" si="106"/>
         <v>0.97751000016597789</v>
       </c>
-      <c r="AT77" s="2">
+      <c r="AT77">
         <v>36173.199999999997</v>
       </c>
       <c r="AU77">
@@ -10635,7 +10737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>904.59583959999998</v>
       </c>
@@ -10702,7 +10804,7 @@
       <c r="V78">
         <v>20095.7</v>
       </c>
-      <c r="X78" s="2">
+      <c r="X78">
         <v>17866.3</v>
       </c>
       <c r="Y78">
@@ -10772,7 +10874,7 @@
         <f t="shared" si="106"/>
         <v>1</v>
       </c>
-      <c r="AT78" s="2">
+      <c r="AT78">
         <v>17866.3</v>
       </c>
       <c r="AU78">
@@ -10843,15 +10945,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X79"/>
+      <c r="AT79"/>
+    </row>
+    <row r="80" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X80"/>
+      <c r="AT80"/>
+    </row>
+    <row r="81" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
         <v>22</v>
       </c>
       <c r="B81" t="s">
         <v>127</v>
       </c>
+      <c r="X81"/>
+      <c r="AT81"/>
     </row>
-    <row r="82" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>723.49619859999996</v>
       </c>
@@ -10918,7 +11030,7 @@
       <c r="V82">
         <v>20986.799999999999</v>
       </c>
-      <c r="X82" s="2">
+      <c r="X82">
         <v>17171.2</v>
       </c>
       <c r="Y82">
@@ -10988,7 +11100,7 @@
         <f t="shared" si="106"/>
         <v>1</v>
       </c>
-      <c r="AT82" s="2">
+      <c r="AT82">
         <v>17171.2</v>
       </c>
       <c r="AU82">
@@ -11023,43 +11135,43 @@
         <v>1</v>
       </c>
       <c r="BF82">
-        <f t="shared" ref="BF82:BF94" si="117">N82/AU82</f>
+        <f t="shared" ref="BF82:BF86" si="117">N82/AU82</f>
         <v>1</v>
       </c>
       <c r="BG82">
-        <f t="shared" ref="BG82:BG94" si="118">O82/AV82</f>
+        <f t="shared" ref="BG82:BG86" si="118">O82/AV82</f>
         <v>1</v>
       </c>
       <c r="BH82">
-        <f t="shared" ref="BH82:BH94" si="119">P82/AW82</f>
+        <f t="shared" ref="BH82:BH86" si="119">P82/AW82</f>
         <v>1</v>
       </c>
       <c r="BI82">
-        <f t="shared" ref="BI82:BI94" si="120">Q82/AX82</f>
+        <f t="shared" ref="BI82:BI86" si="120">Q82/AX82</f>
         <v>1</v>
       </c>
       <c r="BJ82">
-        <f t="shared" ref="BJ82:BJ94" si="121">R82/AY82</f>
+        <f t="shared" ref="BJ82:BJ86" si="121">R82/AY82</f>
         <v>1</v>
       </c>
       <c r="BK82">
-        <f t="shared" ref="BK82:BK94" si="122">S82/AZ82</f>
+        <f t="shared" ref="BK82:BK86" si="122">S82/AZ82</f>
         <v>1</v>
       </c>
       <c r="BL82">
-        <f t="shared" ref="BL82:BL94" si="123">T82/BA82</f>
+        <f t="shared" ref="BL82:BL86" si="123">T82/BA82</f>
         <v>1</v>
       </c>
       <c r="BM82">
-        <f t="shared" ref="BM82:BM94" si="124">U82/BB82</f>
+        <f t="shared" ref="BM82:BM86" si="124">U82/BB82</f>
         <v>1</v>
       </c>
       <c r="BN82">
-        <f t="shared" ref="BN82:BN94" si="125">V82/BC82</f>
+        <f t="shared" ref="BN82:BN86" si="125">V82/BC82</f>
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>751.52860199999998</v>
       </c>
@@ -11126,7 +11238,7 @@
       <c r="V83">
         <v>43518.400000000001</v>
       </c>
-      <c r="X83" s="2">
+      <c r="X83">
         <v>39817.699999999997</v>
       </c>
       <c r="Y83">
@@ -11196,7 +11308,7 @@
         <f t="shared" si="106"/>
         <v>0.93878070510372913</v>
       </c>
-      <c r="AT83" s="2">
+      <c r="AT83">
         <v>37366.9</v>
       </c>
       <c r="AU83">
@@ -11267,7 +11379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>779.55995710000002</v>
       </c>
@@ -11334,7 +11446,7 @@
       <c r="V84">
         <v>76734</v>
       </c>
-      <c r="X84" s="2">
+      <c r="X84">
         <v>56033.2</v>
       </c>
       <c r="Y84">
@@ -11404,7 +11516,7 @@
         <f t="shared" si="106"/>
         <v>0.97838185886688045</v>
       </c>
-      <c r="AT84" s="2">
+      <c r="AT84">
         <v>55000.9</v>
       </c>
       <c r="AU84">
@@ -11475,7 +11587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>803.56062240000006</v>
       </c>
@@ -11542,7 +11654,7 @@
       <c r="V85">
         <v>54620.6</v>
       </c>
-      <c r="X85" s="2">
+      <c r="X85">
         <v>49087.3</v>
       </c>
       <c r="Y85">
@@ -11612,7 +11724,7 @@
         <f t="shared" si="106"/>
         <v>0.9951427655263887</v>
       </c>
-      <c r="AT85" s="2">
+      <c r="AT85">
         <v>48950.6</v>
       </c>
       <c r="AU85">
@@ -11683,7 +11795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A86">
         <v>829.57662979999998</v>
       </c>
@@ -11750,7 +11862,7 @@
       <c r="V86">
         <v>20533.099999999999</v>
       </c>
-      <c r="X86" s="2">
+      <c r="X86">
         <v>18651.7</v>
       </c>
       <c r="Y86">
@@ -11820,7 +11932,7 @@
         <f t="shared" si="106"/>
         <v>1</v>
       </c>
-      <c r="AT86" s="2">
+      <c r="AT86">
         <v>18651.7</v>
       </c>
       <c r="AU86">
@@ -11891,15 +12003,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X87"/>
+      <c r="AT87"/>
+    </row>
+    <row r="88" spans="1:66" x14ac:dyDescent="0.5">
+      <c r="X88"/>
+      <c r="AT88"/>
+    </row>
+    <row r="89" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
         <v>22</v>
       </c>
       <c r="B89" t="s">
         <v>138</v>
       </c>
+      <c r="X89"/>
+      <c r="AT89"/>
     </row>
-    <row r="90" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A90">
         <v>754.60591780000004</v>
       </c>
@@ -11966,7 +12088,7 @@
       <c r="V90">
         <v>85877.7</v>
       </c>
-      <c r="X90" s="2">
+      <c r="X90">
         <v>64343.8</v>
       </c>
       <c r="Y90">
@@ -12036,7 +12158,7 @@
         <f t="shared" si="106"/>
         <v>1</v>
       </c>
-      <c r="AT90" s="2">
+      <c r="AT90">
         <v>64343.8</v>
       </c>
       <c r="AU90">
@@ -12107,7 +12229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A91">
         <v>782.63734360000001</v>
       </c>
@@ -12174,7 +12296,7 @@
       <c r="V91">
         <v>63236.6</v>
       </c>
-      <c r="X91" s="2">
+      <c r="X91">
         <v>39752.6</v>
       </c>
       <c r="Y91">
@@ -12244,7 +12366,7 @@
         <f t="shared" si="106"/>
         <v>1</v>
       </c>
-      <c r="AT91" s="2">
+      <c r="AT91">
         <v>39752.6</v>
       </c>
       <c r="AU91">
@@ -12315,7 +12437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A92">
         <v>810.66858509999997</v>
       </c>
@@ -12382,7 +12504,7 @@
       <c r="V92">
         <v>26260.9</v>
       </c>
-      <c r="X92" s="2">
+      <c r="X92">
         <v>18798.400000000001</v>
       </c>
       <c r="Y92">
@@ -12452,7 +12574,7 @@
         <f t="shared" si="106"/>
         <v>1</v>
       </c>
-      <c r="AT92" s="2">
+      <c r="AT92">
         <v>18798.400000000001</v>
       </c>
       <c r="AU92">
@@ -12523,7 +12645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A93">
         <v>838.69952009999997</v>
       </c>
@@ -12590,7 +12712,7 @@
       <c r="V93">
         <v>50872.9</v>
       </c>
-      <c r="X93" s="2">
+      <c r="X93">
         <v>40100.800000000003</v>
       </c>
       <c r="Y93">
@@ -12660,7 +12782,7 @@
         <f t="shared" si="106"/>
         <v>1</v>
       </c>
-      <c r="AT93" s="2">
+      <c r="AT93">
         <v>40100.800000000003</v>
       </c>
       <c r="AU93">
@@ -12731,7 +12853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:66" x14ac:dyDescent="0.5">
       <c r="A94">
         <v>866.73117749999994</v>
       </c>
@@ -12798,7 +12920,7 @@
       <c r="V94">
         <v>68706.2</v>
       </c>
-      <c r="X94" s="2">
+      <c r="X94">
         <v>50045.4</v>
       </c>
       <c r="Y94">
@@ -12868,7 +12990,7 @@
         <f t="shared" si="106"/>
         <v>1</v>
       </c>
-      <c r="AT94" s="2">
+      <c r="AT94">
         <v>50045.4</v>
       </c>
       <c r="AU94">
@@ -12943,4 +13065,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: use ppm instead of 0.005 for isocorrection tol
</commit_message>
<xml_diff>
--- a/test_resources/t_sim/reference/Reference.xlsx
+++ b/test_resources/t_sim/reference/Reference.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="406">
   <si>
     <t>PRM</t>
   </si>
@@ -1249,9 +1249,6 @@
   <si>
     <t>pydevd warning: Computing repr of get_no_res_masterscan (MasterScan) was slow (took 0.84s)</t>
   </si>
-  <si>
-    <t xml:space="preserve">O10 N1 P1 D5 </t>
-  </si>
 </sst>
 </file>
 
@@ -31085,25 +31082,25 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>60208.5</v>
+        <v>60149</v>
       </c>
       <c r="O7">
-        <v>75937.2</v>
+        <v>75885.3</v>
       </c>
       <c r="P7">
         <v>116647.1</v>
       </c>
       <c r="Q7">
-        <v>96927.2</v>
+        <v>96883.5</v>
       </c>
       <c r="R7">
         <v>145236.1</v>
       </c>
       <c r="S7">
-        <v>103648.4</v>
+        <v>103578.9</v>
       </c>
       <c r="T7">
-        <v>118161.3</v>
+        <v>118072</v>
       </c>
       <c r="U7">
         <v>141952.5</v>
@@ -31112,7 +31109,7 @@
         <v>53563.9</v>
       </c>
       <c r="W7">
-        <v>96068.5</v>
+        <v>96020.800000000003</v>
       </c>
     </row>
     <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.5">
@@ -31499,34 +31496,34 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>58387.5</v>
+        <v>58322.8</v>
       </c>
       <c r="O13">
-        <v>71490.2</v>
+        <v>71411.5</v>
       </c>
       <c r="P13">
-        <v>104530.8</v>
+        <v>104416.8</v>
       </c>
       <c r="Q13">
-        <v>87983.5</v>
+        <v>87885.3</v>
       </c>
       <c r="R13">
-        <v>128359.1</v>
+        <v>128249.2</v>
       </c>
       <c r="S13">
-        <v>95546.1</v>
+        <v>95438.399999999994</v>
       </c>
       <c r="T13">
-        <v>98391</v>
+        <v>98265.8</v>
       </c>
       <c r="U13">
-        <v>131139.4</v>
+        <v>130980.6</v>
       </c>
       <c r="V13">
-        <v>49738.1</v>
+        <v>49691.199999999997</v>
       </c>
       <c r="W13">
-        <v>90054</v>
+        <v>89966.5</v>
       </c>
     </row>
     <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.5">
@@ -31706,34 +31703,34 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>88837.1</v>
+        <v>88747.8</v>
       </c>
       <c r="O16">
-        <v>106448.7</v>
+        <v>106347.2</v>
       </c>
       <c r="P16">
-        <v>151347.9</v>
+        <v>151151.4</v>
       </c>
       <c r="Q16">
-        <v>129400.5</v>
+        <v>129225.7</v>
       </c>
       <c r="R16">
-        <v>186811.6</v>
+        <v>186605.9</v>
       </c>
       <c r="S16">
-        <v>140244.6</v>
+        <v>140099.5</v>
       </c>
       <c r="T16">
-        <v>166196.1</v>
+        <v>165995.70000000001</v>
       </c>
       <c r="U16">
-        <v>209058.8</v>
+        <v>208792.8</v>
       </c>
       <c r="V16">
         <v>78146.100000000006</v>
       </c>
       <c r="W16">
-        <v>140368.4</v>
+        <v>140237.1</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.5">
@@ -32008,7 +32005,7 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <v>44991.9</v>
+        <v>44947.7</v>
       </c>
       <c r="O23">
         <v>53058.9</v>
@@ -32304,40 +32301,40 @@
         <v>-0.24</v>
       </c>
       <c r="L30">
-        <v>342.4</v>
+        <v>363.3</v>
       </c>
       <c r="M30">
         <v>0</v>
       </c>
       <c r="N30">
-        <v>12441.8</v>
+        <v>12708.2</v>
       </c>
       <c r="O30">
-        <v>16564.3</v>
+        <v>16795.3</v>
       </c>
       <c r="P30">
-        <v>20738.3</v>
+        <v>22061.5</v>
       </c>
       <c r="Q30">
-        <v>19177.599999999999</v>
+        <v>20601.7</v>
       </c>
       <c r="R30">
-        <v>38347.5</v>
+        <v>38898</v>
       </c>
       <c r="S30">
-        <v>23760.400000000001</v>
+        <v>24172.9</v>
       </c>
       <c r="T30">
-        <v>20846.099999999999</v>
+        <v>21605.9</v>
       </c>
       <c r="U30">
-        <v>35259.4</v>
+        <v>36352.199999999997</v>
       </c>
       <c r="V30">
-        <v>6620.8</v>
+        <v>7085.3</v>
       </c>
       <c r="W30">
-        <v>12333.8</v>
+        <v>12548.2</v>
       </c>
     </row>
     <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.5">
@@ -33393,34 +33390,34 @@
         <v>0</v>
       </c>
       <c r="N51">
-        <v>37521.9</v>
+        <v>37924.6</v>
       </c>
       <c r="O51">
-        <v>46170.5</v>
+        <v>46626.6</v>
       </c>
       <c r="P51">
-        <v>80733.600000000006</v>
+        <v>81583</v>
       </c>
       <c r="Q51">
-        <v>75907</v>
+        <v>76685.899999999994</v>
       </c>
       <c r="R51">
-        <v>114040.3</v>
+        <v>115314.8</v>
       </c>
       <c r="S51">
-        <v>75071.199999999997</v>
+        <v>75843.7</v>
       </c>
       <c r="T51">
-        <v>90624.8</v>
+        <v>91595.199999999997</v>
       </c>
       <c r="U51">
-        <v>116186.5</v>
+        <v>117483.3</v>
       </c>
       <c r="V51">
-        <v>22065.200000000001</v>
+        <v>22284.799999999999</v>
       </c>
       <c r="W51">
-        <v>41549.5</v>
+        <v>41972.800000000003</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.5">
@@ -33464,34 +33461,34 @@
         <v>0</v>
       </c>
       <c r="N52">
-        <v>20931.8</v>
+        <v>21130</v>
       </c>
       <c r="O52">
-        <v>25902</v>
+        <v>26191.5</v>
       </c>
       <c r="P52">
-        <v>39486.199999999997</v>
+        <v>39906.6</v>
       </c>
       <c r="Q52">
-        <v>37471.5</v>
+        <v>37870.5</v>
       </c>
       <c r="R52">
-        <v>57312.4</v>
+        <v>57923.3</v>
       </c>
       <c r="S52">
-        <v>35788.699999999997</v>
+        <v>36358.400000000001</v>
       </c>
       <c r="T52">
-        <v>44062.2</v>
+        <v>44492.4</v>
       </c>
       <c r="U52">
-        <v>60102.3</v>
+        <v>60783.199999999997</v>
       </c>
       <c r="V52">
         <v>12082.8</v>
       </c>
       <c r="W52">
-        <v>22324.6</v>
+        <v>22565.9</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.5">
@@ -33627,10 +33624,10 @@
         <v>0</v>
       </c>
       <c r="N57">
-        <v>24925.9</v>
+        <v>25135.5</v>
       </c>
       <c r="O57">
-        <v>30107.7</v>
+        <v>30453.5</v>
       </c>
       <c r="P57">
         <v>45975.6</v>
@@ -33639,22 +33636,22 @@
         <v>42161.3</v>
       </c>
       <c r="R57">
-        <v>77303.399999999994</v>
+        <v>78070.3</v>
       </c>
       <c r="S57">
-        <v>47505.5</v>
+        <v>47979.3</v>
       </c>
       <c r="T57">
-        <v>55850</v>
+        <v>56383.8</v>
       </c>
       <c r="U57">
-        <v>68823.100000000006</v>
+        <v>69565</v>
       </c>
       <c r="V57">
         <v>12417.7</v>
       </c>
       <c r="W57">
-        <v>23297.5</v>
+        <v>23506.6</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.5">
@@ -33920,7 +33917,7 @@
         <v>-1.45</v>
       </c>
       <c r="L64">
-        <v>413.8</v>
+        <v>426.4</v>
       </c>
       <c r="M64">
         <v>0</v>
@@ -34133,34 +34130,34 @@
         <v>0</v>
       </c>
       <c r="N67">
-        <v>25031.599999999999</v>
+        <v>25300.7</v>
       </c>
       <c r="O67">
-        <v>31683.5</v>
+        <v>32047.4</v>
       </c>
       <c r="P67">
-        <v>45874.9</v>
+        <v>46467.3</v>
       </c>
       <c r="Q67">
-        <v>47188.5</v>
+        <v>47733</v>
       </c>
       <c r="R67">
-        <v>72411</v>
+        <v>73281.399999999994</v>
       </c>
       <c r="S67">
-        <v>48054.8</v>
+        <v>48641.3</v>
       </c>
       <c r="T67">
-        <v>47749.7</v>
+        <v>48312.4</v>
       </c>
       <c r="U67">
-        <v>73341.399999999994</v>
+        <v>74104</v>
       </c>
       <c r="V67">
-        <v>13201.6</v>
+        <v>13423.3</v>
       </c>
       <c r="W67">
-        <v>22783.5</v>
+        <v>23083.599999999999</v>
       </c>
     </row>
     <row r="68" spans="1:23" hidden="1" x14ac:dyDescent="0.5">
@@ -34411,7 +34408,7 @@
         <v>4317.3999999999996</v>
       </c>
       <c r="P71">
-        <v>11345.5</v>
+        <v>11405.4</v>
       </c>
       <c r="Q71">
         <v>11486</v>
@@ -34467,7 +34464,7 @@
         <v>-1.49</v>
       </c>
       <c r="L72">
-        <v>349.6</v>
+        <v>370.7</v>
       </c>
       <c r="M72">
         <v>0</v>
@@ -34538,40 +34535,40 @@
         <v>-0.24</v>
       </c>
       <c r="L73">
-        <v>342.4</v>
+        <v>363.3</v>
       </c>
       <c r="M73">
         <v>0</v>
       </c>
       <c r="N73">
-        <v>12441.8</v>
+        <v>12708.2</v>
       </c>
       <c r="O73">
-        <v>16564.3</v>
+        <v>16795.3</v>
       </c>
       <c r="P73">
-        <v>20738.3</v>
+        <v>22061.5</v>
       </c>
       <c r="Q73">
-        <v>19177.599999999999</v>
+        <v>20601.7</v>
       </c>
       <c r="R73">
-        <v>38347.5</v>
+        <v>38898</v>
       </c>
       <c r="S73">
-        <v>23760.400000000001</v>
+        <v>24172.9</v>
       </c>
       <c r="T73">
-        <v>20846.099999999999</v>
+        <v>21605.9</v>
       </c>
       <c r="U73">
-        <v>35259.4</v>
+        <v>36352.199999999997</v>
       </c>
       <c r="V73">
-        <v>6620.8</v>
+        <v>7085.3</v>
       </c>
       <c r="W73">
-        <v>12333.8</v>
+        <v>12548.2</v>
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.5">
@@ -34630,40 +34627,40 @@
         <v>0.75</v>
       </c>
       <c r="L77">
-        <v>320.89999999999998</v>
+        <v>308.2</v>
       </c>
       <c r="M77">
         <v>0</v>
       </c>
       <c r="N77">
-        <v>9118.2000000000007</v>
+        <v>9420.5</v>
       </c>
       <c r="O77">
-        <v>11218.8</v>
+        <v>11628.6</v>
       </c>
       <c r="P77">
-        <v>13408.6</v>
+        <v>13782.8</v>
       </c>
       <c r="Q77">
-        <v>11565.3</v>
+        <v>11865.1</v>
       </c>
       <c r="R77">
-        <v>14492.1</v>
+        <v>15174.7</v>
       </c>
       <c r="S77">
-        <v>9846</v>
+        <v>10281.799999999999</v>
       </c>
       <c r="T77">
-        <v>13007.1</v>
+        <v>13500.3</v>
       </c>
       <c r="U77">
-        <v>16463.7</v>
+        <v>17115.099999999999</v>
       </c>
       <c r="V77">
-        <v>8752.5</v>
+        <v>8982</v>
       </c>
       <c r="W77">
-        <v>14876.6</v>
+        <v>15271.8</v>
       </c>
     </row>
     <row r="78" spans="1:23" hidden="1" x14ac:dyDescent="0.5">
@@ -34902,7 +34899,7 @@
         <v>-1.1599999999999999</v>
       </c>
       <c r="L81">
-        <v>658.5</v>
+        <v>619</v>
       </c>
       <c r="M81">
         <v>0</v>
@@ -35313,7 +35310,7 @@
         <v>4.91</v>
       </c>
       <c r="L87">
-        <v>231.8</v>
+        <v>304.89999999999998</v>
       </c>
       <c r="M87">
         <v>0</v>
@@ -35470,7 +35467,7 @@
         <v>0</v>
       </c>
       <c r="S89">
-        <v>275.10000000000002</v>
+        <v>274.89999999999998</v>
       </c>
       <c r="T89">
         <v>0</v>
@@ -36351,10 +36348,10 @@
         <v>4813.5</v>
       </c>
       <c r="P102">
-        <v>23159.5</v>
+        <v>19907.099999999999</v>
       </c>
       <c r="Q102">
-        <v>20750.2</v>
+        <v>17687</v>
       </c>
       <c r="R102">
         <v>10252.200000000001</v>
@@ -36363,10 +36360,10 @@
         <v>7606.9</v>
       </c>
       <c r="T102">
-        <v>15749.1</v>
+        <v>13907.2</v>
       </c>
       <c r="U102">
-        <v>21131.9</v>
+        <v>18693.099999999999</v>
       </c>
       <c r="V102">
         <v>2921.5</v>
@@ -37602,7 +37599,7 @@
         <v>0</v>
       </c>
       <c r="N123">
-        <v>66369.3</v>
+        <v>66326.100000000006</v>
       </c>
       <c r="O123">
         <v>82212.800000000003</v>
@@ -37629,7 +37626,7 @@
         <v>54321</v>
       </c>
       <c r="W123">
-        <v>94462</v>
+        <v>94382.1</v>
       </c>
     </row>
     <row r="124" spans="1:23" hidden="1" x14ac:dyDescent="0.5">
@@ -37901,7 +37898,7 @@
         <v>0</v>
       </c>
       <c r="V127">
-        <v>146</v>
+        <v>145.1</v>
       </c>
       <c r="W127">
         <v>0</v>
@@ -38836,10 +38833,10 @@
         <v>66912.7</v>
       </c>
       <c r="P146">
-        <v>39950.6</v>
+        <v>41646.400000000001</v>
       </c>
       <c r="Q146">
-        <v>42105.5</v>
+        <v>43702.7</v>
       </c>
       <c r="R146">
         <v>118406.39999999999</v>
@@ -38848,10 +38845,10 @@
         <v>71700.5</v>
       </c>
       <c r="T146">
-        <v>71375.100000000006</v>
+        <v>72335.600000000006</v>
       </c>
       <c r="U146">
-        <v>94375.7</v>
+        <v>95647.4</v>
       </c>
       <c r="V146">
         <v>39174.400000000001</v>
@@ -39534,7 +39531,7 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="L159">
-        <v>639.9</v>
+        <v>619.79999999999995</v>
       </c>
       <c r="M159">
         <v>0</v>
@@ -39877,7 +39874,7 @@
         <v>0.19</v>
       </c>
       <c r="L164">
-        <v>45.9</v>
+        <v>146.4</v>
       </c>
       <c r="M164">
         <v>0</v>
@@ -39945,40 +39942,40 @@
         <v>0.75</v>
       </c>
       <c r="L165">
-        <v>320.89999999999998</v>
+        <v>308.2</v>
       </c>
       <c r="M165">
         <v>0</v>
       </c>
       <c r="N165">
-        <v>9118.2000000000007</v>
+        <v>9420.5</v>
       </c>
       <c r="O165">
-        <v>11218.8</v>
+        <v>11628.6</v>
       </c>
       <c r="P165">
-        <v>13408.6</v>
+        <v>13782.8</v>
       </c>
       <c r="Q165">
-        <v>11565.3</v>
+        <v>11865.1</v>
       </c>
       <c r="R165">
-        <v>14492.1</v>
+        <v>15174.7</v>
       </c>
       <c r="S165">
-        <v>9846</v>
+        <v>10281.799999999999</v>
       </c>
       <c r="T165">
-        <v>13007.1</v>
+        <v>13500.3</v>
       </c>
       <c r="U165">
-        <v>16463.7</v>
+        <v>17115.099999999999</v>
       </c>
       <c r="V165">
-        <v>8752.5</v>
+        <v>8982</v>
       </c>
       <c r="W165">
-        <v>14876.6</v>
+        <v>15271.8</v>
       </c>
     </row>
     <row r="166" spans="1:23" hidden="1" x14ac:dyDescent="0.5">
@@ -40099,7 +40096,7 @@
         <v>8573.9</v>
       </c>
       <c r="R167">
-        <v>6825.3</v>
+        <v>7147.3</v>
       </c>
       <c r="S167">
         <v>7664.2</v>
@@ -40149,7 +40146,7 @@
         <v>4.17</v>
       </c>
       <c r="L168">
-        <v>484</v>
+        <v>462.2</v>
       </c>
       <c r="M168">
         <v>0</v>
@@ -40529,67 +40526,70 @@
       </c>
     </row>
     <row r="174" spans="1:23" hidden="1" x14ac:dyDescent="0.5">
-      <c r="B174" t="s">
-        <v>406</v>
+      <c r="B174">
+        <v>797.51429667968705</v>
       </c>
       <c r="C174" t="s">
+        <v>387</v>
+      </c>
+      <c r="D174" t="s">
         <v>127</v>
       </c>
-      <c r="D174">
+      <c r="E174">
         <v>37</v>
       </c>
-      <c r="E174">
+      <c r="F174">
         <v>6</v>
       </c>
-      <c r="F174">
-        <v>0</v>
-      </c>
-      <c r="G174" t="s">
+      <c r="G174">
+        <v>0</v>
+      </c>
+      <c r="H174" t="s">
         <v>388</v>
       </c>
-      <c r="H174" t="s">
+      <c r="I174" t="s">
         <v>26</v>
       </c>
-      <c r="I174" t="s">
+      <c r="J174" t="s">
         <v>57</v>
       </c>
-      <c r="J174">
+      <c r="K174">
         <v>1.01</v>
       </c>
-      <c r="K174">
+      <c r="L174">
         <v>175.7</v>
       </c>
-      <c r="L174">
-        <v>0</v>
-      </c>
       <c r="M174">
+        <v>0</v>
+      </c>
+      <c r="N174">
         <v>704.6</v>
       </c>
-      <c r="N174">
+      <c r="O174">
         <v>817</v>
       </c>
-      <c r="O174">
+      <c r="P174">
         <v>1344.3</v>
       </c>
-      <c r="P174">
+      <c r="Q174">
         <v>1126.7</v>
       </c>
-      <c r="Q174">
+      <c r="R174">
         <v>1728.6</v>
       </c>
-      <c r="R174">
+      <c r="S174">
         <v>1116.8</v>
       </c>
-      <c r="S174">
+      <c r="T174">
         <v>1058.2</v>
       </c>
-      <c r="T174">
+      <c r="U174">
         <v>1837.1</v>
       </c>
-      <c r="U174">
+      <c r="V174">
         <v>478.7</v>
       </c>
-      <c r="V174">
+      <c r="W174">
         <v>915</v>
       </c>
     </row>
@@ -40832,7 +40832,7 @@
         <v>4.91</v>
       </c>
       <c r="L178">
-        <v>231.8</v>
+        <v>304.89999999999998</v>
       </c>
       <c r="M178">
         <v>0</v>
@@ -41612,8 +41612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL66" workbookViewId="0">
-      <selection activeCell="BI103" sqref="BI103"/>
+    <sheetView tabSelected="1" topLeftCell="AL19" workbookViewId="0">
+      <selection activeCell="BI1" sqref="BI1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -42050,25 +42050,25 @@
         <v>0</v>
       </c>
       <c r="AJ5">
-        <v>60208.5</v>
+        <v>60149</v>
       </c>
       <c r="AK5">
-        <v>75937.2</v>
+        <v>75885.3</v>
       </c>
       <c r="AL5">
         <v>116647.1</v>
       </c>
       <c r="AM5">
-        <v>96927.2</v>
+        <v>96883.5</v>
       </c>
       <c r="AN5">
         <v>145236.1</v>
       </c>
       <c r="AO5">
-        <v>103648.4</v>
+        <v>103578.9</v>
       </c>
       <c r="AP5">
-        <v>118161.3</v>
+        <v>118072</v>
       </c>
       <c r="AQ5">
         <v>141952.5</v>
@@ -42077,7 +42077,7 @@
         <v>53563.9</v>
       </c>
       <c r="AS5">
-        <v>96068.5</v>
+        <v>96020.800000000003</v>
       </c>
       <c r="AU5">
         <v>0</v>
@@ -42087,11 +42087,11 @@
       </c>
       <c r="AW5">
         <f t="shared" ref="AW5:AW68" si="1">AJ5/M5</f>
-        <v>1.0004552924423116</v>
+        <v>0.99946660994897074</v>
       </c>
       <c r="AX5">
         <f t="shared" ref="AX5:AX68" si="2">AK5/N5</f>
-        <v>1.0003148328422029</v>
+        <v>0.99963115817649872</v>
       </c>
       <c r="AY5">
         <f t="shared" ref="AY5:AY68" si="3">AL5/O5</f>
@@ -42099,7 +42099,7 @@
       </c>
       <c r="AZ5">
         <f t="shared" ref="AZ5:AZ68" si="4">AM5/P5</f>
-        <v>1.0002084472741908</v>
+        <v>0.99975749945824344</v>
       </c>
       <c r="BA5">
         <f t="shared" ref="BA5:BA68" si="5">AN5/Q5</f>
@@ -42107,11 +42107,11 @@
       </c>
       <c r="BB5">
         <f t="shared" ref="BB5:BB68" si="6">AO5/R5</f>
-        <v>1.000290489228254</v>
+        <v>0.99961975828593974</v>
       </c>
       <c r="BC5">
         <f t="shared" ref="BC5:BC68" si="7">AP5/S5</f>
-        <v>1.000293752634885</v>
+        <v>0.9995377840384807</v>
       </c>
       <c r="BD5">
         <f t="shared" ref="BD5:BD68" si="8">AQ5/T5</f>
@@ -42123,7 +42123,7 @@
       </c>
       <c r="BF5">
         <f t="shared" ref="BF5:BF68" si="10">AS5/V5</f>
-        <v>1.0002290557178033</v>
+        <v>0.99973242127511153</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.5">
@@ -42410,34 +42410,34 @@
         <v>0</v>
       </c>
       <c r="AJ7">
-        <v>58387.5</v>
+        <v>58322.8</v>
       </c>
       <c r="AK7">
-        <v>71490.2</v>
+        <v>71411.5</v>
       </c>
       <c r="AL7">
-        <v>104530.8</v>
+        <v>104416.8</v>
       </c>
       <c r="AM7">
-        <v>87983.5</v>
+        <v>87885.3</v>
       </c>
       <c r="AN7">
-        <v>128359.1</v>
+        <v>128249.2</v>
       </c>
       <c r="AO7">
-        <v>95546.1</v>
+        <v>95438.399999999994</v>
       </c>
       <c r="AP7">
-        <v>98391</v>
+        <v>98265.8</v>
       </c>
       <c r="AQ7">
-        <v>131139.4</v>
+        <v>130980.6</v>
       </c>
       <c r="AR7">
-        <v>49738.1</v>
+        <v>49691.199999999997</v>
       </c>
       <c r="AS7">
-        <v>90054</v>
+        <v>89966.5</v>
       </c>
       <c r="AU7">
         <v>0</v>
@@ -42447,43 +42447,43 @@
       </c>
       <c r="AW7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.99889188610575896</v>
       </c>
       <c r="AX7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.99889914981354089</v>
       </c>
       <c r="AY7">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.99890941234545227</v>
       </c>
       <c r="AZ7">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.9988838816368979</v>
       </c>
       <c r="BA7">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.99914380826914484</v>
       </c>
       <c r="BB7">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.99887279543592034</v>
       </c>
       <c r="BC7">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.99872752589159586</v>
       </c>
       <c r="BD7">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0.99878907483182022</v>
       </c>
       <c r="BE7">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.99905706088491519</v>
       </c>
       <c r="BF7">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.99902836076132095</v>
       </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.5">
@@ -42590,34 +42590,34 @@
         <v>0</v>
       </c>
       <c r="AJ8">
-        <v>88837.1</v>
+        <v>88747.8</v>
       </c>
       <c r="AK8">
-        <v>106448.7</v>
+        <v>106347.2</v>
       </c>
       <c r="AL8">
-        <v>151347.9</v>
+        <v>151151.4</v>
       </c>
       <c r="AM8">
-        <v>129400.5</v>
+        <v>129225.7</v>
       </c>
       <c r="AN8">
-        <v>186811.6</v>
+        <v>186605.9</v>
       </c>
       <c r="AO8">
-        <v>140244.6</v>
+        <v>140099.5</v>
       </c>
       <c r="AP8">
-        <v>166196.1</v>
+        <v>165995.70000000001</v>
       </c>
       <c r="AQ8">
-        <v>209058.8</v>
+        <v>208792.8</v>
       </c>
       <c r="AR8">
         <v>78146.100000000006</v>
       </c>
       <c r="AS8">
-        <v>140368.4</v>
+        <v>140237.1</v>
       </c>
       <c r="AU8">
         <v>0</v>
@@ -42627,35 +42627,35 @@
       </c>
       <c r="AW8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.99899478933913866</v>
       </c>
       <c r="AX8">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.9990464890599885</v>
       </c>
       <c r="AY8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.99870166682193806</v>
       </c>
       <c r="AZ8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.99864915514236807</v>
       </c>
       <c r="BA8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.99889889064704751</v>
       </c>
       <c r="BB8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.99896537905915805</v>
       </c>
       <c r="BC8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.99879419553166415</v>
       </c>
       <c r="BD8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0.99872763069528769</v>
       </c>
       <c r="BE8">
         <f t="shared" si="9"/>
@@ -42663,7 +42663,7 @@
       </c>
       <c r="BF8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.99906460428415522</v>
       </c>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.5">
@@ -43145,7 +43145,7 @@
         <v>0</v>
       </c>
       <c r="AJ14">
-        <v>44991.9</v>
+        <v>44947.7</v>
       </c>
       <c r="AK14">
         <v>53058.9</v>
@@ -43182,7 +43182,7 @@
       </c>
       <c r="AW14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.99901760094594794</v>
       </c>
       <c r="AX14">
         <f t="shared" si="2"/>
@@ -45028,34 +45028,34 @@
         <v>0</v>
       </c>
       <c r="AJ33">
-        <v>37521.9</v>
+        <v>37924.6</v>
       </c>
       <c r="AK33">
-        <v>46170.5</v>
+        <v>46626.6</v>
       </c>
       <c r="AL33">
-        <v>80733.600000000006</v>
+        <v>81583</v>
       </c>
       <c r="AM33">
-        <v>75907</v>
+        <v>76685.899999999994</v>
       </c>
       <c r="AN33">
-        <v>114040.3</v>
+        <v>115314.8</v>
       </c>
       <c r="AO33">
-        <v>75071.199999999997</v>
+        <v>75843.7</v>
       </c>
       <c r="AP33">
-        <v>90624.8</v>
+        <v>91595.199999999997</v>
       </c>
       <c r="AQ33">
-        <v>116186.5</v>
+        <v>117483.3</v>
       </c>
       <c r="AR33">
-        <v>22065.200000000001</v>
+        <v>22284.799999999999</v>
       </c>
       <c r="AS33">
-        <v>41549.5</v>
+        <v>41972.800000000003</v>
       </c>
       <c r="AU33">
         <v>0</v>
@@ -45065,43 +45065,43 @@
       </c>
       <c r="AW33">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0107323989456822</v>
       </c>
       <c r="AX33">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0098786021377286</v>
       </c>
       <c r="AY33">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.0105210222261858</v>
       </c>
       <c r="AZ33">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.0102612407287865</v>
       </c>
       <c r="BA33">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>1.011175873791984</v>
       </c>
       <c r="BB33">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>1.0102902311405706</v>
       </c>
       <c r="BC33">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>1.0107078857001615</v>
       </c>
       <c r="BD33">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>1.0111613655631249</v>
       </c>
       <c r="BE33">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>1.0099523231151315</v>
       </c>
       <c r="BF33">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>1.0101878482292206</v>
       </c>
     </row>
     <row r="34" spans="1:58" x14ac:dyDescent="0.5">
@@ -45208,34 +45208,34 @@
         <v>0</v>
       </c>
       <c r="AJ34">
-        <v>20931.8</v>
+        <v>21130</v>
       </c>
       <c r="AK34">
-        <v>25902</v>
+        <v>26191.5</v>
       </c>
       <c r="AL34">
-        <v>39486.199999999997</v>
+        <v>39906.6</v>
       </c>
       <c r="AM34">
-        <v>37471.5</v>
+        <v>37870.5</v>
       </c>
       <c r="AN34">
-        <v>57312.4</v>
+        <v>57923.3</v>
       </c>
       <c r="AO34">
-        <v>35788.699999999997</v>
+        <v>36358.400000000001</v>
       </c>
       <c r="AP34">
-        <v>44062.2</v>
+        <v>44492.4</v>
       </c>
       <c r="AQ34">
-        <v>60102.3</v>
+        <v>60783.199999999997</v>
       </c>
       <c r="AR34">
         <v>12082.8</v>
       </c>
       <c r="AS34">
-        <v>22324.6</v>
+        <v>22565.9</v>
       </c>
       <c r="AU34">
         <v>0</v>
@@ -45245,35 +45245,35 @@
       </c>
       <c r="AW34">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0094688464441663</v>
       </c>
       <c r="AX34">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0111767431086403</v>
       </c>
       <c r="AY34">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.01064675760139</v>
       </c>
       <c r="AZ34">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.0106480925503383</v>
       </c>
       <c r="BA34">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>1.0106591243779706</v>
       </c>
       <c r="BB34">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>1.0159184323543466</v>
       </c>
       <c r="BC34">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>1.0097634707300136</v>
       </c>
       <c r="BD34">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>1.0113290173587366</v>
       </c>
       <c r="BE34">
         <f t="shared" si="9"/>
@@ -45281,7 +45281,7 @@
       </c>
       <c r="BF34">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>1.0108087042992933</v>
       </c>
     </row>
     <row r="35" spans="1:58" x14ac:dyDescent="0.5">
@@ -45595,10 +45595,10 @@
         <v>0</v>
       </c>
       <c r="AJ39">
-        <v>24925.9</v>
+        <v>25135.5</v>
       </c>
       <c r="AK39">
-        <v>30107.7</v>
+        <v>30453.5</v>
       </c>
       <c r="AL39">
         <v>45975.6</v>
@@ -45607,22 +45607,22 @@
         <v>42161.3</v>
       </c>
       <c r="AN39">
-        <v>77303.399999999994</v>
+        <v>78070.3</v>
       </c>
       <c r="AO39">
-        <v>47505.5</v>
+        <v>47979.3</v>
       </c>
       <c r="AP39">
-        <v>55850</v>
+        <v>56383.8</v>
       </c>
       <c r="AQ39">
-        <v>68823.100000000006</v>
+        <v>69565</v>
       </c>
       <c r="AR39">
         <v>12417.7</v>
       </c>
       <c r="AS39">
-        <v>23297.5</v>
+        <v>23506.6</v>
       </c>
       <c r="AU39">
         <v>0</v>
@@ -45632,11 +45632,11 @@
       </c>
       <c r="AW39">
         <f t="shared" si="1"/>
-        <v>0.9916611963159675</v>
+        <v>1</v>
       </c>
       <c r="AX39">
         <f t="shared" si="2"/>
-        <v>0.98864498333524886</v>
+        <v>1</v>
       </c>
       <c r="AY39">
         <f t="shared" si="3"/>
@@ -45648,19 +45648,19 @@
       </c>
       <c r="BA39">
         <f t="shared" si="5"/>
-        <v>0.99017680218982107</v>
+        <v>1</v>
       </c>
       <c r="BB39">
         <f t="shared" si="6"/>
-        <v>0.99012490803325592</v>
+        <v>1</v>
       </c>
       <c r="BC39">
         <f t="shared" si="7"/>
-        <v>0.99053274167402694</v>
+        <v>1</v>
       </c>
       <c r="BD39">
         <f t="shared" si="8"/>
-        <v>0.98933515417235685</v>
+        <v>1</v>
       </c>
       <c r="BE39">
         <f t="shared" si="9"/>
@@ -45668,7 +45668,7 @@
       </c>
       <c r="BF39">
         <f t="shared" si="10"/>
-        <v>0.99110462593484394</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:58" x14ac:dyDescent="0.5">
@@ -46162,34 +46162,34 @@
         <v>0</v>
       </c>
       <c r="AJ45">
-        <v>25031.599999999999</v>
+        <v>25300.7</v>
       </c>
       <c r="AK45">
-        <v>31683.5</v>
+        <v>32047.4</v>
       </c>
       <c r="AL45">
-        <v>45874.9</v>
+        <v>46467.3</v>
       </c>
       <c r="AM45">
-        <v>47188.5</v>
+        <v>47733</v>
       </c>
       <c r="AN45">
-        <v>72411</v>
+        <v>73281.399999999994</v>
       </c>
       <c r="AO45">
-        <v>48054.8</v>
+        <v>48641.3</v>
       </c>
       <c r="AP45">
-        <v>47749.7</v>
+        <v>48312.4</v>
       </c>
       <c r="AQ45">
-        <v>73341.399999999994</v>
+        <v>74104</v>
       </c>
       <c r="AR45">
-        <v>13201.6</v>
+        <v>13423.3</v>
       </c>
       <c r="AS45">
-        <v>22783.5</v>
+        <v>23083.599999999999</v>
       </c>
       <c r="AU45">
         <v>0</v>
@@ -46199,43 +46199,43 @@
       </c>
       <c r="AW45">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0107504114798895</v>
       </c>
       <c r="AX45">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0114854735114491</v>
       </c>
       <c r="AY45">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.0129133796476941</v>
       </c>
       <c r="AZ45">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.0115388283162212</v>
       </c>
       <c r="BA45">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>1.0120202731629171</v>
       </c>
       <c r="BB45">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>1.012204816168208</v>
       </c>
       <c r="BC45">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>1.0117843672316267</v>
       </c>
       <c r="BD45">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>1.010397947134906</v>
       </c>
       <c r="BE45">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>1.0167934189795176</v>
       </c>
       <c r="BF45">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>1.0131718129347993</v>
       </c>
     </row>
     <row r="46" spans="1:58" x14ac:dyDescent="0.5">
@@ -46336,40 +46336,40 @@
         <v>-0.24</v>
       </c>
       <c r="AH46">
-        <v>342.4</v>
+        <v>363.3</v>
       </c>
       <c r="AI46">
         <v>0</v>
       </c>
       <c r="AJ46">
-        <v>12441.8</v>
+        <v>12708.2</v>
       </c>
       <c r="AK46">
-        <v>16564.3</v>
+        <v>16795.3</v>
       </c>
       <c r="AL46">
-        <v>20738.3</v>
+        <v>22061.5</v>
       </c>
       <c r="AM46">
-        <v>19177.599999999999</v>
+        <v>20601.7</v>
       </c>
       <c r="AN46">
-        <v>38347.5</v>
+        <v>38898</v>
       </c>
       <c r="AO46">
-        <v>23760.400000000001</v>
+        <v>24172.9</v>
       </c>
       <c r="AP46">
-        <v>20846.099999999999</v>
+        <v>21605.9</v>
       </c>
       <c r="AQ46">
-        <v>35259.4</v>
+        <v>36352.199999999997</v>
       </c>
       <c r="AR46">
-        <v>6620.8</v>
+        <v>7085.3</v>
       </c>
       <c r="AS46">
-        <v>12333.8</v>
+        <v>12548.2</v>
       </c>
       <c r="AU46">
         <v>0</v>
@@ -46379,43 +46379,43 @@
       </c>
       <c r="AW46">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0214116928418719</v>
       </c>
       <c r="AX46">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0139456542081464</v>
       </c>
       <c r="AY46">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.063804651297358</v>
       </c>
       <c r="AZ46">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.0742585099282498</v>
       </c>
       <c r="BA46">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>1.0143555642479953</v>
       </c>
       <c r="BB46">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>1.0173608188414336</v>
       </c>
       <c r="BC46">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>1.0364480646259973</v>
       </c>
       <c r="BD46">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>1.0309931535987564</v>
       </c>
       <c r="BE46">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>1.0701576848719188</v>
       </c>
       <c r="BF46">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>1.0173831260438795</v>
       </c>
     </row>
     <row r="47" spans="1:58" x14ac:dyDescent="0.5">
@@ -46543,87 +46543,87 @@
         <v>0.75</v>
       </c>
       <c r="AH50">
-        <v>320.89999999999998</v>
+        <v>308.2</v>
       </c>
       <c r="AI50">
         <v>0</v>
       </c>
       <c r="AJ50">
-        <v>9118.2000000000007</v>
+        <v>9420.5</v>
       </c>
       <c r="AK50">
-        <v>11218.8</v>
+        <v>11628.6</v>
       </c>
       <c r="AL50">
-        <v>13408.6</v>
+        <v>13782.8</v>
       </c>
       <c r="AM50">
-        <v>11565.3</v>
+        <v>11865.1</v>
       </c>
       <c r="AN50">
-        <v>14492.1</v>
+        <v>15174.7</v>
       </c>
       <c r="AO50">
-        <v>9846</v>
+        <v>10281.799999999999</v>
       </c>
       <c r="AP50">
-        <v>13007.1</v>
+        <v>13500.3</v>
       </c>
       <c r="AQ50">
-        <v>16463.7</v>
+        <v>17115.099999999999</v>
       </c>
       <c r="AR50">
-        <v>8752.5</v>
+        <v>8982</v>
       </c>
       <c r="AS50">
-        <v>14876.6</v>
+        <v>15271.8</v>
       </c>
       <c r="AU50" s="3">
         <f t="shared" si="11"/>
-        <v>1.0428989275268119</v>
+        <v>1.0016249593760156</v>
       </c>
       <c r="AV50" s="3">
         <v>0</v>
       </c>
       <c r="AW50" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.0331534732732337</v>
       </c>
       <c r="AX50" s="3">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.0365279709059794</v>
       </c>
       <c r="AY50" s="3">
         <f>AL50/O50</f>
-        <v>1</v>
+        <v>1.0279074623748936</v>
       </c>
       <c r="AZ50" s="3">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.0259223712311831</v>
       </c>
       <c r="BA50" s="3">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>1.0471015242787449</v>
       </c>
       <c r="BB50" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>1.0442616290879545</v>
       </c>
       <c r="BC50" s="3">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>1.0379177526120349</v>
       </c>
       <c r="BD50" s="3">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>1.0395658327107513</v>
       </c>
       <c r="BE50" s="3">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>1.0262210796915168</v>
       </c>
       <c r="BF50" s="3">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>1.0265652097925602</v>
       </c>
     </row>
     <row r="51" spans="1:58" x14ac:dyDescent="0.5">
@@ -47828,7 +47828,7 @@
         <v>0</v>
       </c>
       <c r="AJ60">
-        <v>66369.3</v>
+        <v>66326.100000000006</v>
       </c>
       <c r="AK60">
         <v>82212.800000000003</v>
@@ -47855,7 +47855,7 @@
         <v>54321</v>
       </c>
       <c r="AS60">
-        <v>94462</v>
+        <v>94382.1</v>
       </c>
       <c r="AU60">
         <v>0</v>
@@ -47865,7 +47865,7 @@
       </c>
       <c r="AW60">
         <f t="shared" si="1"/>
-        <v>1.0007644914096498</v>
+        <v>1.0001130904452145</v>
       </c>
       <c r="AX60">
         <f t="shared" si="2"/>
@@ -47901,7 +47901,7 @@
       </c>
       <c r="BF60">
         <f t="shared" si="10"/>
-        <v>1.0008465588284219</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:58" x14ac:dyDescent="0.5">
@@ -49662,10 +49662,10 @@
         <v>66912.7</v>
       </c>
       <c r="AL76">
-        <v>39950.6</v>
+        <v>41646.400000000001</v>
       </c>
       <c r="AM76">
-        <v>42105.5</v>
+        <v>43702.7</v>
       </c>
       <c r="AN76">
         <v>118406.39999999999</v>
@@ -49674,10 +49674,10 @@
         <v>71700.5</v>
       </c>
       <c r="AP76">
-        <v>71375.100000000006</v>
+        <v>72335.600000000006</v>
       </c>
       <c r="AQ76">
-        <v>94375.7</v>
+        <v>95647.4</v>
       </c>
       <c r="AR76">
         <v>39174.400000000001</v>
@@ -49701,11 +49701,11 @@
       </c>
       <c r="AY76">
         <f t="shared" si="14"/>
-        <v>0.85051945840074938</v>
+        <v>0.88662181725283151</v>
       </c>
       <c r="AZ76">
         <f t="shared" si="15"/>
-        <v>0.91148888821540375</v>
+        <v>0.94606465746782065</v>
       </c>
       <c r="BA76">
         <f t="shared" si="16"/>
@@ -49717,11 +49717,11 @@
       </c>
       <c r="BC76">
         <f t="shared" si="18"/>
-        <v>0.98763093442554906</v>
+        <v>1.0009215569607992</v>
       </c>
       <c r="BD76">
         <f t="shared" si="19"/>
-        <v>0.98761500724158424</v>
+        <v>1.0009229880534789</v>
       </c>
       <c r="BE76">
         <f t="shared" si="20"/>

</xml_diff>